<commit_message>
vault backup: 2025-12-15 03:39:40
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013DDF17-F549-4497-AA7E-F72404D1C496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664D017-2FCA-48FB-A9DE-DA682F8AE0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10152" yWindow="0" windowWidth="18816" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="5904" yWindow="0" windowWidth="37500" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
   <si>
     <t>Giocatore</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>libro incantesimi</t>
-  </si>
-  <si>
-    <t>2 Gemme 40 m.o. l'una</t>
   </si>
   <si>
     <t>open stuck doors on
@@ -191,18 +188,12 @@
     <t>abiti standard</t>
   </si>
   <si>
-    <t>Tesori</t>
-  </si>
-  <si>
     <t>-1 on NPC reactions, max. 3 retainers, retainer morale 6</t>
   </si>
   <si>
     <t>Abilità</t>
   </si>
   <si>
-    <t>Incantesimi</t>
-  </si>
-  <si>
     <t>1 Livello</t>
   </si>
   <si>
@@ -287,28 +278,25 @@
     <t>3 Livello</t>
   </si>
   <si>
-    <t>Freccie</t>
-  </si>
-  <si>
-    <t>Torcoe</t>
-  </si>
-  <si>
-    <t>Razioni</t>
-  </si>
-  <si>
-    <t>Acqua Santa</t>
-  </si>
-  <si>
-    <t>100 m.o</t>
-  </si>
-  <si>
-    <t>404 m.o.</t>
-  </si>
-  <si>
-    <t>Banca</t>
-  </si>
-  <si>
     <t>THAC0 - CA avversario = Tiro necessario</t>
+  </si>
+  <si>
+    <t>mo</t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>Incantesimi Scelti</t>
+  </si>
+  <si>
+    <t>Monete</t>
+  </si>
+  <si>
+    <t>pp</t>
+  </si>
+  <si>
+    <t>ma</t>
   </si>
 </sst>
 </file>
@@ -493,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,43 +570,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -953,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263CECC3-3302-44DA-8376-3DD3643BBD45}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -981,12 +957,12 @@
       <c r="G1" s="10"/>
       <c r="H1" s="8"/>
       <c r="I1" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
@@ -996,15 +972,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="8"/>
@@ -1014,7 +990,7 @@
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
@@ -1043,13 +1019,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="29" t="s">
         <v>77</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>80</v>
       </c>
       <c r="K4" s="20">
         <v>0</v>
@@ -1064,7 +1040,7 @@
     </row>
     <row r="5" spans="1:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="14"/>
       <c r="K5" s="14" t="s">
@@ -1081,20 +1057,20 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="K6" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
+      <c r="C6" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="K6" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
       <c r="N6" s="6">
         <v>10</v>
       </c>
@@ -1106,20 +1082,20 @@
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="K7" s="41" t="s">
+      <c r="C7" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="K7" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
       <c r="N7" s="6">
         <v>10</v>
       </c>
@@ -1131,20 +1107,20 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="K8" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
+      <c r="C8" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="K8" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
       <c r="N8" s="6">
         <v>10</v>
       </c>
@@ -1156,20 +1132,20 @@
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="K9" s="41" t="s">
+      <c r="C9" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="K9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
       <c r="N9" s="6">
         <v>13</v>
       </c>
@@ -1181,20 +1157,20 @@
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="K10" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
+      <c r="C10" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="K10" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
       <c r="N10" s="6">
         <v>11</v>
       </c>
@@ -1206,25 +1182,25 @@
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="C11" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="7"/>
       <c r="E13" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -1241,17 +1217,17 @@
     </row>
     <row r="14" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="36"/>
       <c r="E14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="H14" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="40"/>
+      <c r="H14" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="34"/>
       <c r="L14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1260,12 +1236,12 @@
       <c r="A15" s="36"/>
       <c r="B15" s="36"/>
       <c r="E15" s="27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="26"/>
       <c r="H15" s="37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I15" s="37">
         <v>11</v>
@@ -1278,13 +1254,13 @@
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="E16" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="H16" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="40">
+      <c r="H16" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="34">
         <v>12</v>
       </c>
       <c r="L16" s="8" t="s">
@@ -1295,15 +1271,15 @@
       <c r="A17" s="36"/>
       <c r="B17" s="36"/>
       <c r="E17" s="27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="26"/>
       <c r="H17" s="37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I17" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>18</v>
@@ -1311,45 +1287,43 @@
     </row>
     <row r="18" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="H18" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="40" t="s">
-        <v>29</v>
+      <c r="H18" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>28</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>88</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B19" s="9"/>
       <c r="E19" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" s="27"/>
       <c r="G19" s="26"/>
       <c r="H19" s="37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I19" s="37"/>
       <c r="L19" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>19</v>
@@ -1357,135 +1331,109 @@
     </row>
     <row r="21" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
+        <v>80</v>
+      </c>
+      <c r="B21" s="1">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
     </row>
     <row r="22" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
+      <c r="A22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
     </row>
     <row r="23" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="9"/>
+      <c r="A23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
       <c r="L23" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
     </row>
     <row r="24" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="L24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="L24" s="3" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="25" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="L25" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="L25" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
+        <v>51</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
       <c r="L26" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
       <c r="L27" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="32">
-        <v>20</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H28" s="31">
-        <v>3</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
       <c r="L28" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="33">
-        <v>5</v>
-      </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="33">
-        <v>10</v>
-      </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-    </row>
-    <row r="31" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>31</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>32</v>
       </c>
       <c r="D32" s="22">
         <v>8</v>
@@ -1523,18 +1471,18 @@
         <v>0</v>
       </c>
       <c r="M32" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="N32" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N32" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="24">
         <v>7</v>
@@ -1576,16 +1524,16 @@
         <v>16</v>
       </c>
       <c r="M33" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:14" ht="18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="24">
         <v>8</v>
@@ -1627,16 +1575,16 @@
         <v>17</v>
       </c>
       <c r="M34" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:14" ht="18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>42</v>
       </c>
       <c r="C35" s="24">
         <v>9</v>
@@ -1678,14 +1626,22 @@
         <v>18</v>
       </c>
       <c r="M35" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA36" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L21:N21"/>
     <mergeCell ref="L22:N22"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="H18:I18"/>
@@ -1701,11 +1657,6 @@
     <mergeCell ref="C8:I8"/>
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C10:I10"/>
-    <mergeCell ref="A14:B17"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L21:N21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-15 10:38:55
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664D017-2FCA-48FB-A9DE-DA682F8AE0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C63C33-11DF-402A-A5E0-4154EC4BAC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5904" yWindow="0" windowWidth="37500" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="5904" yWindow="0" windowWidth="21024" windowHeight="16656" activeTab="1" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scheda" sheetId="1" r:id="rId1"/>
+    <sheet name="Oggetti" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
   <si>
     <t>Giocatore</t>
   </si>
@@ -290,6 +291,9 @@
     <t>Incantesimi Scelti</t>
   </si>
   <si>
+    <t>SLOT</t>
+  </si>
+  <si>
     <t>Monete</t>
   </si>
   <si>
@@ -297,13 +301,28 @@
   </si>
   <si>
     <t>ma</t>
+  </si>
+  <si>
+    <t>Qt.</t>
+  </si>
+  <si>
+    <t>Oggetto</t>
+  </si>
+  <si>
+    <t>Slot</t>
+  </si>
+  <si>
+    <t>Modf.</t>
+  </si>
+  <si>
+    <t>TOTALE:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,8 +432,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,8 +467,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -477,11 +523,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -595,6 +663,39 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -931,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263CECC3-3302-44DA-8376-3DD3643BBD45}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -1302,7 +1403,7 @@
     </row>
     <row r="19" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="9"/>
       <c r="E19" s="27" t="s">
@@ -1320,7 +1421,7 @@
     </row>
     <row r="20" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -1345,7 +1446,7 @@
     </row>
     <row r="22" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1661,4 +1762,323 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7F733B-4F29-4CC7-8875-78DA591CD6C7}">
+  <dimension ref="A1:I84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.21875" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="40">
+        <v>22</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="40">
+        <v>1</v>
+      </c>
+      <c r="H1" s="41"/>
+      <c r="I1" s="40"/>
+    </row>
+    <row r="3" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+    </row>
+    <row r="4" spans="1:9" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+    </row>
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+    </row>
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="48"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+    </row>
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+    </row>
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="48"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+    </row>
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+    </row>
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="48"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+    </row>
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+    </row>
+    <row r="13" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="48"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+    </row>
+    <row r="14" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+    </row>
+    <row r="15" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="46"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+    </row>
+    <row r="16" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+    </row>
+    <row r="17" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="48"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+    </row>
+    <row r="18" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+    </row>
+    <row r="19" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="48"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+    </row>
+    <row r="20" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="51"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+    </row>
+    <row r="21" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="48"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+    </row>
+    <row r="22" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="51"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+    </row>
+    <row r="23" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="48"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+    </row>
+    <row r="24" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="51"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+    </row>
+    <row r="25" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+    </row>
+    <row r="26" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="51"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+    </row>
+    <row r="27" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="48"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+    </row>
+    <row r="28" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="51"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+    </row>
+    <row r="29" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="48"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+    </row>
+    <row r="30" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="51"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+    </row>
+    <row r="31" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="48"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+    </row>
+    <row r="32" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="51"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+    </row>
+    <row r="33" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="48"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+    </row>
+    <row r="34" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="51"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+    </row>
+    <row r="35" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-12-16 00:06:50
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C63C33-11DF-402A-A5E0-4154EC4BAC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F910A-BFA2-4AE0-8B05-105396F12E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5904" yWindow="0" windowWidth="21024" windowHeight="16656" activeTab="1" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="10572" yWindow="0" windowWidth="23244" windowHeight="16656" activeTab="1" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Scheda" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
   <si>
     <t>Giocatore</t>
   </si>
@@ -291,9 +291,6 @@
     <t>Incantesimi Scelti</t>
   </si>
   <si>
-    <t>SLOT</t>
-  </si>
-  <si>
     <t>Monete</t>
   </si>
   <si>
@@ -312,17 +309,74 @@
     <t>Slot</t>
   </si>
   <si>
-    <t>Modf.</t>
-  </si>
-  <si>
-    <t>TOTALE:</t>
+    <t>Anelli, amuleti, pergamene singole, chiavi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armi piccole, torce, pozioni, corda, razioni, monete (ogni 100) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armi medie, armatura leggera, scudo </t>
+  </si>
+  <si>
+    <t>Armi grandi, armatura pesante, scudo grande</t>
+  </si>
+  <si>
+    <t>Forza</t>
+  </si>
+  <si>
+    <t>Slot 1/2</t>
+  </si>
+  <si>
+    <t>Fermo</t>
+  </si>
+  <si>
+    <t>6-8</t>
+  </si>
+  <si>
+    <t>9-12</t>
+  </si>
+  <si>
+    <t>13-15</t>
+  </si>
+  <si>
+    <t>16-17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19+</t>
+  </si>
+  <si>
+    <t>24+</t>
+  </si>
+  <si>
+    <t>27+</t>
+  </si>
+  <si>
+    <t>30+</t>
+  </si>
+  <si>
+    <t>33+</t>
+  </si>
+  <si>
+    <t>36+</t>
+  </si>
+  <si>
+    <t>Esempio</t>
+  </si>
+  <si>
+    <t>Formula: 20 + (modificatore FOR × 2)</t>
+  </si>
+  <si>
+    <t>Note/Usi/Cariche</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,21 +488,33 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <name val="Aptos Narrow"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos ExtraBold"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Aptos ExtraBold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos ExtraBold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,18 +535,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -528,8 +600,118 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -541,15 +723,19 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -645,6 +831,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -656,51 +855,128 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos ExtraBold"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -711,6 +987,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DFE39CCD-A3A0-411F-9284-620A9D624E2B}" name="Tabella2" displayName="Tabella2" ref="G33:J39" totalsRowShown="0" headerRowDxfId="0" dataDxfId="9">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FED5B1ED-E990-4C12-98A3-45B4AFC7099E}" name="Forza" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{52EEBE46-E85D-48C6-BE0A-0F79720C2ECC}" name="Slot" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{87D2820E-9CDF-4235-9FAE-7EBD8ADA922E}" name="Slot 1/2" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{766288AF-7925-485A-A044-7F27BEF8F717}" name="Fermo" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CAFD96BD-AC57-4A6D-8FEF-C762082851F6}" name="Tabella4" displayName="Tabella4" ref="A34:F37" headerRowCount="0" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{3E8D725F-3420-49DC-9272-6DA174F28A43}" name="Slot" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{13EC648B-9BE7-4801-A3AA-676F4FF28666}" name="Esempi" headerRowDxfId="14" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{67909A8B-E635-48E7-8B76-822A015EE759}" name="*" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{7DCA39A4-AC31-4C9E-AA06-E60D0283313A}" name="*2" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{A4FB9732-EFA4-4140-856E-7175744505F7}" name="'-2" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{C20E2C16-5E16-4933-9CBF-A83B68B83E64}" name="'-3" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1158,20 +1460,20 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="K6" s="35" t="s">
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="K6" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
       <c r="N6" s="6">
         <v>10</v>
       </c>
@@ -1183,20 +1485,20 @@
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="K7" s="35" t="s">
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="K7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
       <c r="N7" s="6">
         <v>10</v>
       </c>
@@ -1208,20 +1510,20 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="K8" s="35" t="s">
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="K8" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
       <c r="N8" s="6">
         <v>10</v>
       </c>
@@ -1233,20 +1535,20 @@
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="K9" s="35" t="s">
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="K9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
       <c r="N9" s="6">
         <v>13</v>
       </c>
@@ -1258,20 +1560,20 @@
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="K10" s="35" t="s">
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="K10" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
       <c r="N10" s="6">
         <v>11</v>
       </c>
@@ -1283,15 +1585,15 @@
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
     </row>
     <row r="12" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1317,34 +1619,34 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="36"/>
+      <c r="B14" s="35"/>
       <c r="E14" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="H14" s="34" t="s">
+      <c r="H14" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="34"/>
+      <c r="I14" s="39"/>
       <c r="L14" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
       <c r="E15" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15" s="36">
         <v>11</v>
       </c>
       <c r="L15" s="8" t="s">
@@ -1352,16 +1654,16 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="E16" s="7" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="34">
+      <c r="I16" s="39">
         <v>12</v>
       </c>
       <c r="L16" s="8" t="s">
@@ -1369,17 +1671,17 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="E17" s="27" t="s">
         <v>69</v>
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="26"/>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="I17" s="37" t="s">
+      <c r="I17" s="36" t="s">
         <v>28</v>
       </c>
       <c r="L17" s="8" t="s">
@@ -1391,10 +1693,10 @@
         <v>70</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="39" t="s">
         <v>28</v>
       </c>
       <c r="L18" s="8" t="s">
@@ -1403,7 +1705,7 @@
     </row>
     <row r="19" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="9"/>
       <c r="E19" s="27" t="s">
@@ -1411,17 +1713,17 @@
       </c>
       <c r="F19" s="27"/>
       <c r="G19" s="26"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="I19" s="37"/>
+      <c r="I19" s="36"/>
       <c r="L19" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -1440,20 +1742,20 @@
       <c r="E21" t="s">
         <v>79</v>
       </c>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
     </row>
     <row r="22" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
     </row>
     <row r="23" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
@@ -1734,15 +2036,10 @@
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="AA36" s="38"/>
+      <c r="AA36"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A14:B17"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L21:N21"/>
     <mergeCell ref="L22:N22"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="H18:I18"/>
@@ -1758,6 +2055,11 @@
     <mergeCell ref="C8:I8"/>
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C10:I10"/>
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L21:N21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1766,281 +2068,566 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7F733B-4F29-4CC7-8875-78DA591CD6C7}">
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.21875" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="32" customWidth="1"/>
+    <col min="3" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C1" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="40">
-        <v>22</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" s="40">
+    <row r="1" spans="1:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+    </row>
+    <row r="2" spans="1:10" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="60">
         <v>1</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="40"/>
-    </row>
-    <row r="3" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-    </row>
-    <row r="4" spans="1:9" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-    </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-    </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-    </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-    </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-    </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="48"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-    </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-    </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="48"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-    </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+    </row>
+    <row r="4" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="61">
+        <f>A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+    </row>
+    <row r="5" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="62">
+        <v>3</v>
+      </c>
+      <c r="B5"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="61">
+        <v>4</v>
+      </c>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+    </row>
+    <row r="7" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="62">
+        <v>5</v>
+      </c>
+      <c r="B7"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="61">
+        <v>6</v>
+      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+    </row>
+    <row r="9" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="62">
+        <v>7</v>
+      </c>
+      <c r="B9"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="61">
+        <v>8</v>
+      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+    </row>
+    <row r="11" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="62">
+        <v>9</v>
+      </c>
+      <c r="B11"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="63">
+        <v>10</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
-    </row>
-    <row r="13" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="48"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-    </row>
-    <row r="14" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-    </row>
-    <row r="15" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-    </row>
-    <row r="16" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-    </row>
-    <row r="17" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="48"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-    </row>
-    <row r="18" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-    </row>
-    <row r="19" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="48"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-    </row>
-    <row r="20" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-    </row>
-    <row r="21" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="48"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-    </row>
-    <row r="22" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+    </row>
+    <row r="13" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="64">
+        <v>11</v>
+      </c>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+    </row>
+    <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="65">
+        <v>12</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+    </row>
+    <row r="15" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="66">
+        <v>13</v>
+      </c>
+      <c r="B15"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="61">
+        <v>14</v>
+      </c>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+    </row>
+    <row r="17" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="66">
+        <v>15</v>
+      </c>
+      <c r="B17"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+    </row>
+    <row r="18" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="61">
+        <v>16</v>
+      </c>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+    </row>
+    <row r="19" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="66">
+        <v>17</v>
+      </c>
+      <c r="B19"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+    </row>
+    <row r="20" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="61">
+        <v>18</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+    </row>
+    <row r="21" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="66">
+        <v>19</v>
+      </c>
+      <c r="B21"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="63">
+        <v>20</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
-    </row>
-    <row r="23" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="48"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-    </row>
-    <row r="24" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-    </row>
-    <row r="25" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-    </row>
-    <row r="26" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-    </row>
-    <row r="27" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="48"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-    </row>
-    <row r="28" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="51"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-    </row>
-    <row r="29" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="48"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-    </row>
-    <row r="30" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-    </row>
-    <row r="31" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="48"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-    </row>
-    <row r="32" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-    </row>
-    <row r="33" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="48"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-    </row>
-    <row r="34" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="51"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-    </row>
-    <row r="35" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="41" t="s">
+      <c r="G22" s="51"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+    </row>
+    <row r="23" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="66">
+        <v>21</v>
+      </c>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+    </row>
+    <row r="24" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="65">
+        <v>22</v>
+      </c>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+    </row>
+    <row r="25" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="66">
+        <v>23</v>
+      </c>
+      <c r="B25"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+    </row>
+    <row r="26" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="61">
+        <v>24</v>
+      </c>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+    </row>
+    <row r="27" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="66">
+        <v>25</v>
+      </c>
+      <c r="B27"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+    </row>
+    <row r="28" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="61">
+        <v>26</v>
+      </c>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
+    </row>
+    <row r="29" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="66">
+        <v>27</v>
+      </c>
+      <c r="B29"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+    </row>
+    <row r="30" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="61">
+        <v>28</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+    </row>
+    <row r="31" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="67">
+        <v>29</v>
+      </c>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+    </row>
+    <row r="32" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="J33" s="54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>0</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="52">
+        <v>3</v>
+      </c>
+      <c r="H34" s="1">
+        <v>14</v>
+      </c>
+      <c r="I34" s="1">
+        <v>4</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35" s="1">
+        <v>18</v>
+      </c>
+      <c r="I35" s="1">
+        <v>5</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>2</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="1">
+        <v>20</v>
+      </c>
+      <c r="I36" s="1">
+        <v>6</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>3</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="1">
+        <v>22</v>
+      </c>
+      <c r="I37" s="1">
+        <v>7</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" s="1">
+        <v>24</v>
+      </c>
+      <c r="I38" s="1">
+        <v>8</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="1">
+        <v>26</v>
+      </c>
+      <c r="I39" s="1">
+        <v>9</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2069,16 +2656,12 @@
     <row r="74" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="75" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="76" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-12-16 00:55:41
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F910A-BFA2-4AE0-8B05-105396F12E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5849A470-A00D-4085-B724-713879FA7E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10572" yWindow="0" windowWidth="23244" windowHeight="16656" activeTab="1" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
   <si>
     <t>Giocatore</t>
   </si>
@@ -312,15 +312,6 @@
     <t>Anelli, amuleti, pergamene singole, chiavi</t>
   </si>
   <si>
-    <t xml:space="preserve">Armi piccole, torce, pozioni, corda, razioni, monete (ogni 100) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armi medie, armatura leggera, scudo </t>
-  </si>
-  <si>
-    <t>Armi grandi, armatura pesante, scudo grande</t>
-  </si>
-  <si>
     <t>Forza</t>
   </si>
   <si>
@@ -370,13 +361,25 @@
   </si>
   <si>
     <t>Note/Usi/Cariche</t>
+  </si>
+  <si>
+    <t>Armi medie, armatura leggera, scudo , arco corto, balestra l.</t>
+  </si>
+  <si>
+    <t>Armi grandi, armatura pesante, scudo grande, arco l., balestra p.</t>
+  </si>
+  <si>
+    <t>Ogni 100 mo</t>
+  </si>
+  <si>
+    <t>Armi piccole, torce, pozioni, corda, faretra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +508,13 @@
       <color theme="1"/>
       <name val="Aptos ExtraBold"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
@@ -735,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -890,35 +900,77 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -944,18 +996,6 @@
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -990,7 +1030,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DFE39CCD-A3A0-411F-9284-620A9D624E2B}" name="Tabella2" displayName="Tabella2" ref="G33:J39" totalsRowShown="0" headerRowDxfId="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DFE39CCD-A3A0-411F-9284-620A9D624E2B}" name="Tabella2" displayName="Tabella2" ref="G33:J39" totalsRowShown="0" headerRowDxfId="4" dataDxfId="9">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{FED5B1ED-E990-4C12-98A3-45B4AFC7099E}" name="Forza" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{52EEBE46-E85D-48C6-BE0A-0F79720C2ECC}" name="Slot" dataDxfId="12"/>
@@ -1002,14 +1042,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CAFD96BD-AC57-4A6D-8FEF-C762082851F6}" name="Tabella4" displayName="Tabella4" ref="A34:F37" headerRowCount="0" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CAFD96BD-AC57-4A6D-8FEF-C762082851F6}" name="Tabella4" displayName="Tabella4" ref="A34:F38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3E8D725F-3420-49DC-9272-6DA174F28A43}" name="Slot" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{13EC648B-9BE7-4801-A3AA-676F4FF28666}" name="Esempi" headerRowDxfId="14" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{67909A8B-E635-48E7-8B76-822A015EE759}" name="*" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{7DCA39A4-AC31-4C9E-AA06-E60D0283313A}" name="*2" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{A4FB9732-EFA4-4140-856E-7175744505F7}" name="'-2" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{C20E2C16-5E16-4933-9CBF-A83B68B83E64}" name="'-3" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3E8D725F-3420-49DC-9272-6DA174F28A43}" name="Slot" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{13EC648B-9BE7-4801-A3AA-676F4FF28666}" name="Esempi" headerRowDxfId="14" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{67909A8B-E635-48E7-8B76-822A015EE759}" name="*" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{7DCA39A4-AC31-4C9E-AA06-E60D0283313A}" name="*2" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A4FB9732-EFA4-4140-856E-7175744505F7}" name="'-2" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{C20E2C16-5E16-4933-9CBF-A83B68B83E64}" name="'-3" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2071,7 +2111,7 @@
   <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2097,7 +2137,7 @@
         <v>88</v>
       </c>
       <c r="G1" s="59" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H1" s="42"/>
       <c r="I1" s="42"/>
@@ -2462,33 +2502,33 @@
         <v>88</v>
       </c>
       <c r="B33" s="53" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C33" s="53"/>
       <c r="D33" s="53"/>
       <c r="E33" s="53"/>
       <c r="F33" s="53"/>
       <c r="G33" s="54" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H33" s="54" t="s">
         <v>88</v>
       </c>
       <c r="I33" s="54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J33" s="54" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>0</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="3"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -2502,22 +2542,22 @@
         <v>4</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="3"/>
+      <c r="B35" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="69"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H35" s="1">
         <v>18</v>
@@ -2526,22 +2566,22 @@
         <v>5</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="3"/>
+      <c r="B36" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="69"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="52" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H36" s="1">
         <v>20</v>
@@ -2550,22 +2590,22 @@
         <v>6</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>3</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="3"/>
+      <c r="B37" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="69"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="52" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H37" s="1">
         <v>22</v>
@@ -2574,18 +2614,22 @@
         <v>7</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="3"/>
+      <c r="A38" s="1">
+        <v>1</v>
+      </c>
+      <c r="B38" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="69"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="52" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H38" s="1">
         <v>24</v>
@@ -2594,12 +2638,12 @@
         <v>8</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
@@ -2607,7 +2651,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="52" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H39" s="1">
         <v>26</v>
@@ -2616,7 +2660,7 @@
         <v>9</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2658,7 +2702,7 @@
     <row r="76" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-16 18:49:34
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85817E7B-6F3E-446A-ACF8-043E2659429B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DEA29F-5C56-41AD-AA32-72C07BF886F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10644" yWindow="0" windowWidth="25152" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="24504" yWindow="0" windowWidth="17868" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Fighter A" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="156">
   <si>
     <t>Giocatore</t>
   </si>
@@ -491,6 +491,21 @@
   </si>
   <si>
     <t>Guerriero Corazzato Arciere</t>
+  </si>
+  <si>
+    <t>Ascia due mani</t>
+  </si>
+  <si>
+    <t>Arco lungo</t>
+  </si>
+  <si>
+    <t>Ascia/pugnale + Scudo</t>
+  </si>
+  <si>
+    <t>Combinazioni</t>
+  </si>
+  <si>
+    <t>Ritirata difensiva, mezzo movimento, no attacco</t>
   </si>
 </sst>
 </file>
@@ -499,7 +514,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -1031,7 +1046,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1070,21 +1085,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1117,13 +1131,7 @@
     <xf numFmtId="0" fontId="16" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1143,239 +1151,239 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1384,18 +1392,9 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1414,7 +1413,47 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1432,37 +1471,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1495,26 +1503,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DFE39CCD-A3A0-411F-9284-620A9D624E2B}" name="Tabella2" displayName="Tabella2" ref="G33:J39" totalsRowShown="0" headerRowDxfId="4" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DFE39CCD-A3A0-411F-9284-620A9D624E2B}" name="Tabella2" displayName="Tabella2" ref="G33:J39" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FED5B1ED-E990-4C12-98A3-45B4AFC7099E}" name="Forza" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{52EEBE46-E85D-48C6-BE0A-0F79720C2ECC}" name="Slot" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{87D2820E-9CDF-4235-9FAE-7EBD8ADA922E}" name="Slot 1/2" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{766288AF-7925-485A-A044-7F27BEF8F717}" name="Fermo" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{FED5B1ED-E990-4C12-98A3-45B4AFC7099E}" name="Forza" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{52EEBE46-E85D-48C6-BE0A-0F79720C2ECC}" name="Slot" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{87D2820E-9CDF-4235-9FAE-7EBD8ADA922E}" name="Slot 1/2" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{766288AF-7925-485A-A044-7F27BEF8F717}" name="Fermo" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CAFD96BD-AC57-4A6D-8FEF-C762082851F6}" name="Tabella4" displayName="Tabella4" ref="A34:F38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CAFD96BD-AC57-4A6D-8FEF-C762082851F6}" name="Tabella4" displayName="Tabella4" ref="A34:F38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3E8D725F-3420-49DC-9272-6DA174F28A43}" name="Slot" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{13EC648B-9BE7-4801-A3AA-676F4FF28666}" name="Esempi" headerRowDxfId="14" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{67909A8B-E635-48E7-8B76-822A015EE759}" name="*" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{7DCA39A4-AC31-4C9E-AA06-E60D0283313A}" name="*2" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{A4FB9732-EFA4-4140-856E-7175744505F7}" name="'-2" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{C20E2C16-5E16-4933-9CBF-A83B68B83E64}" name="'-3" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{3E8D725F-3420-49DC-9272-6DA174F28A43}" name="Slot" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{13EC648B-9BE7-4801-A3AA-676F4FF28666}" name="Esempi" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{67909A8B-E635-48E7-8B76-822A015EE759}" name="*" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7DCA39A4-AC31-4C9E-AA06-E60D0283313A}" name="*2" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A4FB9732-EFA4-4140-856E-7175744505F7}" name="'-2" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C20E2C16-5E16-4933-9CBF-A83B68B83E64}" name="'-3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1839,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D6BBBE-C9DF-4D21-98BF-29E96594E7D0}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1854,834 +1862,639 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="118" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="101" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="99"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="103" t="s">
+      <c r="H1" s="82"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="104" t="s">
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="O1" s="99"/>
-      <c r="P1" s="105"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="88"/>
     </row>
     <row r="2" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="89" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="109" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
         <v>134</v>
       </c>
-      <c r="H2" s="110"/>
-      <c r="I2" s="117" t="s">
+      <c r="H2" s="93"/>
+      <c r="I2" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="108"/>
-      <c r="K2" s="111" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="107" t="s">
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="107"/>
-      <c r="P2" s="113"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="1:16" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="51"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="45"/>
     </row>
     <row r="4" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="47">
         <v>0</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="54"/>
-      <c r="F4" s="56">
+      <c r="E4" s="1"/>
+      <c r="F4" s="49">
         <v>24</v>
       </c>
-      <c r="G4" s="121" t="s">
+      <c r="G4" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="57" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="58">
+      <c r="L4" s="1"/>
+      <c r="M4" s="51">
         <v>1</v>
       </c>
-      <c r="N4" s="54"/>
-      <c r="O4" s="55" t="s">
+      <c r="N4" s="1"/>
+      <c r="O4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="115">
+      <c r="P4" s="98">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="52" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
       <c r="M5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="60"/>
+      <c r="P5" s="53"/>
     </row>
     <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="94">
+      <c r="A6" s="80">
         <v>17</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="56">
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="49">
         <v>2</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="62" t="s">
+      <c r="K6" s="49"/>
+      <c r="M6" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="63">
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="54">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="94">
+      <c r="A7" s="80">
         <v>14</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="109" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="56">
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="49">
         <v>1</v>
       </c>
-      <c r="K7" s="56"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="62" t="s">
+      <c r="K7" s="49"/>
+      <c r="M7" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63">
+      <c r="N7" s="110"/>
+      <c r="O7" s="110"/>
+      <c r="P7" s="54">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="94">
+      <c r="A8" s="80">
         <v>11</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="56">
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="49">
         <v>0</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="62" t="s">
+      <c r="K8" s="49"/>
+      <c r="M8" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="63">
-        <v>14</v>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="54">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="94">
+      <c r="A9" s="80">
         <v>7</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="56">
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="49">
         <v>-1</v>
       </c>
-      <c r="K9" s="56"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="62" t="s">
+      <c r="K9" s="49"/>
+      <c r="M9" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="63">
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="54">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="94">
+      <c r="A10" s="80">
         <v>4</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="109" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="56">
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="49">
         <v>-2</v>
       </c>
-      <c r="K10" s="56"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="62" t="s">
+      <c r="K10" s="49"/>
+      <c r="M10" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="63">
+      <c r="N10" s="110"/>
+      <c r="O10" s="110"/>
+      <c r="P10" s="54">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="94">
+      <c r="A11" s="80">
         <v>10</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="56">
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="49">
         <v>0</v>
       </c>
-      <c r="K11" s="56"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="64"/>
+      <c r="K11" s="49"/>
+      <c r="P11" s="55"/>
     </row>
     <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="64"/>
+      <c r="A12" s="56"/>
+      <c r="P12" s="55"/>
     </row>
     <row r="13" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="48"/>
+      <c r="C13" s="41"/>
       <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="67" t="s">
+      <c r="H13" s="41"/>
+      <c r="I13" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="67" t="s">
+      <c r="K13" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
       <c r="N13" s="4" t="s">
         <v>79</v>
       </c>
       <c r="O13" s="5"/>
-      <c r="P13" s="68"/>
+      <c r="P13" s="59"/>
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="44" t="s">
+      <c r="B14" s="112"/>
+      <c r="E14" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="71" t="s">
+      <c r="F14" s="41"/>
+      <c r="H14" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="72">
+      <c r="I14" s="61">
         <v>20</v>
       </c>
-      <c r="J14" s="73">
+      <c r="J14" s="1">
         <v>6</v>
       </c>
-      <c r="K14" s="73">
+      <c r="K14" s="1">
         <f>I14/5</f>
         <v>4</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48" t="s">
+      <c r="N14" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O14" s="48"/>
-      <c r="P14" s="51"/>
+      <c r="P14" s="45"/>
     </row>
     <row r="15" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="69"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="74" t="s">
+      <c r="A15" s="111"/>
+      <c r="B15" s="112"/>
+      <c r="E15" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76" t="s">
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="77">
+      <c r="I15" s="65">
         <v>60</v>
       </c>
-      <c r="J15" s="77">
+      <c r="J15" s="65">
         <v>18</v>
       </c>
-      <c r="K15" s="77">
+      <c r="K15" s="65">
         <f t="shared" ref="K15:K18" si="0">I15/5</f>
         <v>12</v>
       </c>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48" t="s">
+      <c r="N15" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="O15" s="48"/>
-      <c r="P15" s="51"/>
+      <c r="P15" s="45"/>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="69"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="44" t="s">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112"/>
+      <c r="E16" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="71" t="s">
+      <c r="F16" s="41"/>
+      <c r="H16" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I16" s="72">
+      <c r="I16" s="61">
         <v>60</v>
       </c>
-      <c r="J16" s="73">
+      <c r="J16" s="1">
         <v>18</v>
       </c>
-      <c r="K16" s="73">
+      <c r="K16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48" t="s">
+      <c r="N16" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="O16" s="48"/>
-      <c r="P16" s="51"/>
+      <c r="P16" s="45"/>
     </row>
     <row r="17" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="69"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="74" t="s">
+      <c r="A17" s="111"/>
+      <c r="B17" s="112"/>
+      <c r="E17" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="76" t="s">
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="77">
+      <c r="I17" s="65">
         <v>10</v>
       </c>
-      <c r="J17" s="77">
+      <c r="J17" s="65">
         <v>3</v>
       </c>
-      <c r="K17" s="77">
+      <c r="K17" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48" t="s">
+      <c r="N17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O17" s="48"/>
-      <c r="P17" s="51"/>
+      <c r="P17" s="45"/>
     </row>
     <row r="18" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="44" t="s">
+      <c r="A18" s="44"/>
+      <c r="E18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="71" t="s">
+      <c r="F18" s="41"/>
+      <c r="H18" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="72">
+      <c r="I18" s="61">
         <v>10</v>
       </c>
-      <c r="J18" s="73">
+      <c r="J18" s="1">
         <v>3</v>
       </c>
-      <c r="K18" s="73">
+      <c r="K18" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48" t="s">
+      <c r="N18" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="O18" s="48"/>
-      <c r="P18" s="51"/>
+      <c r="P18" s="45"/>
     </row>
     <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="57" t="s">
         <v>87</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="74" t="s">
+      <c r="E19" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="76" t="s">
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="78" t="s">
+      <c r="I19" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="78" t="s">
+      <c r="J19" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="K19" s="78"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48" t="s">
+      <c r="K19" s="66"/>
+      <c r="N19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="O19" s="48"/>
-      <c r="P19" s="51"/>
+      <c r="P19" s="45"/>
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="79">
+      <c r="B20" s="67">
         <v>0</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="80" t="s">
+      <c r="N20" s="103" t="s">
         <v>149</v>
       </c>
-      <c r="O20" s="80"/>
-      <c r="P20" s="81"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="104"/>
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="79">
+      <c r="B21" s="67">
         <v>500</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="17" t="s">
+      <c r="E21" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="82" t="s">
+      <c r="O21" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="83">
+      <c r="P21" s="69">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="79">
+      <c r="B22" s="67">
         <v>0</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45" t="s">
+      <c r="E22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="82" t="s">
+      <c r="N22" s="3"/>
+      <c r="O22" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="P22" s="83">
+      <c r="P22" s="69">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="79">
+      <c r="B23" s="67">
         <v>0</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="64"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="42"/>
+      <c r="P23" s="55"/>
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45" t="s">
+      <c r="A24" s="56"/>
+      <c r="E24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="64"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="P24" s="55"/>
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45" t="s">
+      <c r="A25" s="56"/>
+      <c r="E25" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="64"/>
+      <c r="P25" s="55"/>
     </row>
     <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="64"/>
+      <c r="E26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P26" s="55"/>
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
+      <c r="A27" s="115" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="114"/>
+      <c r="C27" s="114" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="I27" s="61"/>
       <c r="N27" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O27" s="6"/>
-      <c r="P27" s="60"/>
+      <c r="P27" s="53"/>
     </row>
     <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="120"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45" t="s">
+      <c r="A28" s="116" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="117"/>
+      <c r="C28" s="113">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O28" s="45"/>
-      <c r="P28" s="64"/>
+      <c r="P28" s="55"/>
     </row>
     <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="119"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45" t="s">
+      <c r="A29" s="116" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="117"/>
+      <c r="C29" s="117">
+        <v>2</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O29" s="45"/>
-      <c r="P29" s="64"/>
+      <c r="P29" s="55"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="119"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45" t="s">
+      <c r="A30" s="118" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="117"/>
+      <c r="C30" s="117">
+        <v>2</v>
+      </c>
+      <c r="N30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="45"/>
-      <c r="P30" s="64"/>
+      <c r="P30" s="55"/>
     </row>
     <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="119"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="64"/>
+      <c r="A31" s="118" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="117"/>
+      <c r="C31" s="117">
+        <v>2</v>
+      </c>
+      <c r="P31" s="55"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="64"/>
+      <c r="A32" s="56"/>
+      <c r="P32" s="55"/>
     </row>
     <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="84" t="s">
+      <c r="A33" s="70" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -2725,193 +2538,183 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M33" s="47" t="s">
+      <c r="M33" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="N33" s="47"/>
+      <c r="N33" s="105"/>
       <c r="O33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P33" s="60"/>
+      <c r="P33" s="53"/>
     </row>
     <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="86">
+      <c r="C34" s="72">
         <v>5</v>
       </c>
-      <c r="D34" s="87">
+      <c r="D34" s="73">
         <f>C34+1</f>
         <v>6</v>
       </c>
-      <c r="E34" s="86">
+      <c r="E34" s="72">
         <f t="shared" ref="E34:L34" si="2">D34+1</f>
         <v>7</v>
       </c>
-      <c r="F34" s="87">
+      <c r="F34" s="73">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="G34" s="86">
+      <c r="G34" s="72">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="H34" s="87">
+      <c r="H34" s="73">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I34" s="86">
+      <c r="I34" s="72">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="J34" s="87">
+      <c r="J34" s="73">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="K34" s="86">
+      <c r="K34" s="72">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="L34" s="87">
+      <c r="L34" s="73">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="M34" s="95" t="s">
+      <c r="M34" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="N34" s="95"/>
-      <c r="O34" s="45" t="s">
+      <c r="N34" s="106"/>
+      <c r="O34" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="P34" s="64"/>
+      <c r="P34" s="55"/>
     </row>
     <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="86">
+      <c r="C35" s="72">
         <v>6</v>
       </c>
-      <c r="D35" s="87">
+      <c r="D35" s="73">
         <f t="shared" ref="D35:L36" si="3">C35+1</f>
         <v>7</v>
       </c>
-      <c r="E35" s="86">
+      <c r="E35" s="72">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="F35" s="87">
+      <c r="F35" s="73">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="G35" s="86">
+      <c r="G35" s="72">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="H35" s="87">
+      <c r="H35" s="73">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="I35" s="86">
+      <c r="I35" s="72">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="J35" s="87">
+      <c r="J35" s="73">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="K35" s="86">
+      <c r="K35" s="72">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="L35" s="87">
+      <c r="L35" s="73">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="M35" s="96" t="s">
+      <c r="M35" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="N35" s="96"/>
-      <c r="O35" s="48" t="s">
+      <c r="N35" s="107"/>
+      <c r="O35" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="P35" s="64"/>
+      <c r="P35" s="55"/>
     </row>
     <row r="36" spans="1:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="89" t="s">
+      <c r="B36" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="C36" s="90">
+      <c r="C36" s="76">
         <v>7</v>
       </c>
-      <c r="D36" s="91">
+      <c r="D36" s="77">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="E36" s="90">
+      <c r="E36" s="76">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="F36" s="91">
+      <c r="F36" s="77">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="G36" s="90">
+      <c r="G36" s="76">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="H36" s="91">
+      <c r="H36" s="77">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="I36" s="90">
+      <c r="I36" s="76">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="J36" s="91">
+      <c r="J36" s="77">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="K36" s="90">
+      <c r="K36" s="76">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="L36" s="91">
+      <c r="L36" s="77">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="M36" s="97" t="s">
+      <c r="M36" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="N36" s="97"/>
-      <c r="O36" s="92" t="s">
+      <c r="N36" s="108"/>
+      <c r="O36" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="P36" s="93"/>
+      <c r="P36" s="79"/>
       <c r="AA36"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="C11:I11"/>
     <mergeCell ref="A14:B17"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="M6:O6"/>
@@ -2919,6 +2722,16 @@
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="C8:I8"/>
     <mergeCell ref="M8:O8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -2930,7 +2743,7 @@
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2944,862 +2757,647 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="118" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="99"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="103" t="s">
+      <c r="H1" s="82"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="104" t="s">
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="O1" s="99"/>
-      <c r="P1" s="105"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="88"/>
     </row>
     <row r="2" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="89" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="109" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
         <v>130</v>
       </c>
-      <c r="H2" s="110"/>
-      <c r="I2" s="117" t="s">
+      <c r="H2" s="93"/>
+      <c r="I2" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="108"/>
-      <c r="K2" s="111" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="107" t="s">
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="107"/>
-      <c r="P2" s="113"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="1:16" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="51"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="45"/>
     </row>
     <row r="4" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="47">
         <v>2</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="54"/>
-      <c r="F4" s="56">
+      <c r="E4" s="1"/>
+      <c r="F4" s="49">
         <v>20</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="57" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="58">
+      <c r="L4" s="1"/>
+      <c r="M4" s="51">
         <v>-1</v>
       </c>
-      <c r="N4" s="54"/>
-      <c r="O4" s="55" t="s">
+      <c r="N4" s="1"/>
+      <c r="O4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="115">
+      <c r="P4" s="98">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="52" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
       <c r="M5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="60"/>
+      <c r="P5" s="53"/>
     </row>
     <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="94">
+      <c r="A6" s="80">
         <v>12</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="56">
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="49">
         <v>0</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="62" t="s">
+      <c r="K6" s="49"/>
+      <c r="M6" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="63">
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="54">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="94">
+      <c r="A7" s="80">
         <v>6</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="56">
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="49">
         <v>-1</v>
       </c>
-      <c r="K7" s="56"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="62" t="s">
+      <c r="K7" s="49"/>
+      <c r="M7" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63">
+      <c r="N7" s="110"/>
+      <c r="O7" s="110"/>
+      <c r="P7" s="54">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="94">
+      <c r="A8" s="80">
         <v>12</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="56">
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="49">
         <v>0</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="62" t="s">
+      <c r="K8" s="49"/>
+      <c r="M8" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="63">
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="54">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="94">
+      <c r="A9" s="80">
         <v>7</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="56">
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="49">
         <v>-1</v>
       </c>
-      <c r="K9" s="56"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="62" t="s">
+      <c r="K9" s="49"/>
+      <c r="M9" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="63">
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="54">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="94">
+      <c r="A10" s="80">
         <v>13</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="56">
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="49">
         <v>1</v>
       </c>
-      <c r="K10" s="56"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="62" t="s">
+      <c r="K10" s="49"/>
+      <c r="M10" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="63">
+      <c r="N10" s="110"/>
+      <c r="O10" s="110"/>
+      <c r="P10" s="54">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="94">
+      <c r="A11" s="80">
         <v>9</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="56">
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="49">
         <v>0</v>
       </c>
-      <c r="K11" s="56"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="64"/>
+      <c r="K11" s="49"/>
+      <c r="P11" s="55"/>
     </row>
     <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="64"/>
+      <c r="A12" s="56"/>
+      <c r="P12" s="55"/>
     </row>
     <row r="13" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="48"/>
+      <c r="C13" s="41"/>
       <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="67" t="s">
+      <c r="H13" s="41"/>
+      <c r="I13" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="67" t="s">
+      <c r="K13" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
       <c r="N13" s="4" t="s">
         <v>79</v>
       </c>
       <c r="O13" s="5"/>
-      <c r="P13" s="68"/>
+      <c r="P13" s="59"/>
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="44" t="s">
+      <c r="B14" s="112"/>
+      <c r="E14" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="71" t="s">
+      <c r="F14" s="41"/>
+      <c r="H14" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="72">
+      <c r="I14" s="61">
         <v>20</v>
       </c>
-      <c r="J14" s="73">
+      <c r="J14" s="1">
         <v>6</v>
       </c>
-      <c r="K14" s="73">
+      <c r="K14" s="1">
         <f>I14/5</f>
         <v>4</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48" t="s">
+      <c r="N14" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O14" s="48"/>
-      <c r="P14" s="51"/>
+      <c r="P14" s="45"/>
     </row>
     <row r="15" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="69"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="74" t="s">
+      <c r="A15" s="111"/>
+      <c r="B15" s="112"/>
+      <c r="E15" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76" t="s">
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="77">
+      <c r="I15" s="65">
         <v>60</v>
       </c>
-      <c r="J15" s="77">
+      <c r="J15" s="65">
         <v>18</v>
       </c>
-      <c r="K15" s="77">
+      <c r="K15" s="65">
         <f t="shared" ref="K15:K18" si="0">I15/5</f>
         <v>12</v>
       </c>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48" t="s">
+      <c r="N15" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O15" s="48"/>
-      <c r="P15" s="51"/>
+      <c r="P15" s="45"/>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="69"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="44" t="s">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112"/>
+      <c r="E16" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="71" t="s">
+      <c r="F16" s="41"/>
+      <c r="H16" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I16" s="72">
+      <c r="I16" s="61">
         <v>60</v>
       </c>
-      <c r="J16" s="73">
+      <c r="J16" s="1">
         <v>18</v>
       </c>
-      <c r="K16" s="73">
+      <c r="K16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48" t="s">
+      <c r="N16" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="O16" s="48"/>
-      <c r="P16" s="51"/>
+      <c r="P16" s="45"/>
     </row>
     <row r="17" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="69"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="74" t="s">
+      <c r="A17" s="111"/>
+      <c r="B17" s="112"/>
+      <c r="E17" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="76" t="s">
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="77">
+      <c r="I17" s="65">
         <v>10</v>
       </c>
-      <c r="J17" s="77">
+      <c r="J17" s="65">
         <v>3</v>
       </c>
-      <c r="K17" s="77">
+      <c r="K17" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48" t="s">
+      <c r="N17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O17" s="48"/>
-      <c r="P17" s="51"/>
+      <c r="P17" s="45"/>
     </row>
     <row r="18" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="44" t="s">
+      <c r="A18" s="44"/>
+      <c r="E18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="71" t="s">
+      <c r="F18" s="41"/>
+      <c r="H18" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="72">
+      <c r="I18" s="61">
         <v>10</v>
       </c>
-      <c r="J18" s="73">
+      <c r="J18" s="1">
         <v>3</v>
       </c>
-      <c r="K18" s="73">
+      <c r="K18" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48" t="s">
+      <c r="N18" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O18" s="48"/>
-      <c r="P18" s="51"/>
+      <c r="P18" s="45"/>
     </row>
     <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="57" t="s">
         <v>87</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="74" t="s">
+      <c r="E19" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="76" t="s">
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="78" t="s">
+      <c r="I19" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="78" t="s">
+      <c r="J19" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="K19" s="78"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48" t="s">
+      <c r="K19" s="66"/>
+      <c r="N19" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="O19" s="48"/>
-      <c r="P19" s="51"/>
+      <c r="P19" s="45"/>
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="79">
+      <c r="B20" s="67">
         <v>0</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="80" t="s">
+      <c r="N20" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="O20" s="80"/>
-      <c r="P20" s="81"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="104"/>
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="79">
+      <c r="B21" s="67">
         <v>500</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="17" t="s">
+      <c r="E21" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="82" t="s">
+      <c r="O21" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="83">
+      <c r="P21" s="69">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="79">
+      <c r="B22" s="67">
         <v>0</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45" t="s">
+      <c r="E22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="82" t="s">
+      <c r="N22" s="3"/>
+      <c r="O22" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="P22" s="83">
+      <c r="P22" s="69">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="79">
+      <c r="B23" s="67">
         <v>0</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="64"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="42"/>
+      <c r="P23" s="55"/>
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45" t="s">
+      <c r="A24" s="56"/>
+      <c r="E24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="64"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="P24" s="55"/>
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45" t="s">
+      <c r="A25" s="56"/>
+      <c r="E25" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="64"/>
+      <c r="P25" s="55"/>
     </row>
     <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="64"/>
+      <c r="A26" s="56"/>
+      <c r="P26" s="55"/>
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="57" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="43" t="s">
         <v>126</v>
       </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="49" t="s">
+      <c r="E27" s="43" t="s">
         <v>127</v>
       </c>
       <c r="F27" s="6"/>
-      <c r="G27" s="49" t="s">
+      <c r="G27" s="43" t="s">
         <v>128</v>
       </c>
       <c r="H27" s="6"/>
-      <c r="I27" s="49" t="s">
+      <c r="I27" s="43" t="s">
         <v>129</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
       <c r="N27" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O27" s="6"/>
-      <c r="P27" s="60"/>
+      <c r="P27" s="53"/>
     </row>
     <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="114" t="s">
+      <c r="A28" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45" t="s">
+      <c r="N28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O28" s="45"/>
-      <c r="P28" s="64"/>
+      <c r="P28" s="55"/>
     </row>
     <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="114" t="s">
+      <c r="A29" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45" t="s">
+      <c r="N29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O29" s="45"/>
-      <c r="P29" s="64"/>
+      <c r="P29" s="55"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="114" t="s">
+      <c r="A30" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45" t="s">
+      <c r="N30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="45"/>
-      <c r="P30" s="64"/>
+      <c r="P30" s="55"/>
     </row>
     <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="114" t="s">
+      <c r="A31" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45" t="s">
+      <c r="N31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="O31" s="45"/>
-      <c r="P31" s="64"/>
+      <c r="P31" s="55"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="64"/>
+      <c r="A32" s="56"/>
+      <c r="P32" s="55"/>
     </row>
     <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="84" t="s">
+      <c r="A33" s="70" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -3843,198 +3441,197 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M33" s="47" t="s">
+      <c r="M33" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="N33" s="47"/>
+      <c r="N33" s="105"/>
       <c r="O33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P33" s="60"/>
+      <c r="P33" s="53"/>
     </row>
     <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="86">
+      <c r="C34" s="72">
         <v>8</v>
       </c>
-      <c r="D34" s="87">
+      <c r="D34" s="73">
         <f>C34+1</f>
         <v>9</v>
       </c>
-      <c r="E34" s="86">
+      <c r="E34" s="72">
         <f t="shared" ref="E34:L34" si="2">D34+1</f>
         <v>10</v>
       </c>
-      <c r="F34" s="87">
+      <c r="F34" s="73">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="G34" s="86">
+      <c r="G34" s="72">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="H34" s="87">
+      <c r="H34" s="73">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="I34" s="86">
+      <c r="I34" s="72">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="J34" s="87">
+      <c r="J34" s="73">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="K34" s="86">
+      <c r="K34" s="72">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="L34" s="87">
+      <c r="L34" s="73">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="M34" s="95" t="s">
+      <c r="M34" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="N34" s="95"/>
-      <c r="O34" s="45"/>
-      <c r="P34" s="64"/>
+      <c r="N34" s="106"/>
+      <c r="P34" s="55"/>
     </row>
     <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="86">
+      <c r="C35" s="72">
         <v>8</v>
       </c>
-      <c r="D35" s="87">
+      <c r="D35" s="73">
         <f t="shared" ref="D35:L35" si="3">C35+1</f>
         <v>9</v>
       </c>
-      <c r="E35" s="86">
+      <c r="E35" s="72">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="F35" s="87">
+      <c r="F35" s="73">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="G35" s="86">
+      <c r="G35" s="72">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="H35" s="87">
+      <c r="H35" s="73">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="I35" s="86">
+      <c r="I35" s="72">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="J35" s="87">
+      <c r="J35" s="73">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="K35" s="86">
+      <c r="K35" s="72">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="L35" s="87">
+      <c r="L35" s="73">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="M35" s="96" t="s">
+      <c r="M35" s="107" t="s">
         <v>110</v>
       </c>
-      <c r="N35" s="96"/>
-      <c r="O35" s="48" t="s">
+      <c r="N35" s="107"/>
+      <c r="O35" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P35" s="64"/>
+      <c r="P35" s="55"/>
     </row>
     <row r="36" spans="1:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="89" t="s">
+      <c r="B36" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="90">
+      <c r="C36" s="76">
         <v>9</v>
       </c>
-      <c r="D36" s="91">
+      <c r="D36" s="77">
         <f t="shared" ref="D36:L36" si="4">C36+1</f>
         <v>10</v>
       </c>
-      <c r="E36" s="90">
+      <c r="E36" s="76">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="F36" s="91">
+      <c r="F36" s="77">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="G36" s="90">
+      <c r="G36" s="76">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="H36" s="91">
+      <c r="H36" s="77">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="I36" s="90">
+      <c r="I36" s="76">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="J36" s="91">
+      <c r="J36" s="77">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="K36" s="90">
+      <c r="K36" s="76">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="L36" s="91">
+      <c r="L36" s="77">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="M36" s="97" t="s">
+      <c r="M36" s="108" t="s">
         <v>107</v>
       </c>
-      <c r="N36" s="97"/>
-      <c r="O36" s="92" t="s">
+      <c r="N36" s="108"/>
+      <c r="O36" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="P36" s="93"/>
+      <c r="P36" s="79"/>
       <c r="AA36"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
     <mergeCell ref="M33:N33"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="M35:N35"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="C11:I11"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="A14:B17"/>
-    <mergeCell ref="N20:P20"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4066,13 +3663,13 @@
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>65</v>
       </c>
       <c r="H1" s="15"/>
@@ -4081,36 +3678,36 @@
     </row>
     <row r="2" spans="1:10" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
+      <c r="A3" s="32">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34">
+      <c r="A4" s="33">
         <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35">
+      <c r="A5" s="34">
         <v>3</v>
       </c>
       <c r="B5"/>
@@ -4119,21 +3716,21 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34">
+      <c r="A6" s="33">
         <v>4</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35">
+      <c r="A7" s="34">
         <v>5</v>
       </c>
       <c r="B7"/>
@@ -4142,21 +3739,21 @@
       <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34">
+      <c r="A8" s="33">
         <v>6</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35">
+      <c r="A9" s="34">
         <v>7</v>
       </c>
       <c r="B9"/>
@@ -4165,21 +3762,21 @@
       <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34">
+      <c r="A10" s="33">
         <v>8</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35">
+      <c r="A11" s="34">
         <v>9</v>
       </c>
       <c r="B11"/>
@@ -4188,49 +3785,44 @@
       <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36">
+      <c r="A12" s="35">
         <v>10</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37">
+      <c r="A13" s="34">
         <v>11</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="B13"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38">
+      <c r="A14" s="36">
         <v>12</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39">
+      <c r="A15" s="34">
         <v>13</v>
       </c>
       <c r="B15"/>
@@ -4239,21 +3831,21 @@
       <c r="G15" s="13"/>
     </row>
     <row r="16" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34">
+      <c r="A16" s="33">
         <v>14</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39">
+      <c r="A17" s="34">
         <v>15</v>
       </c>
       <c r="B17"/>
@@ -4262,21 +3854,21 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34">
+      <c r="A18" s="33">
         <v>16</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39">
+      <c r="A19" s="34">
         <v>17</v>
       </c>
       <c r="B19"/>
@@ -4285,21 +3877,21 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34">
+      <c r="A20" s="33">
         <v>18</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39">
+      <c r="A21" s="34">
         <v>19</v>
       </c>
       <c r="B21"/>
@@ -4308,49 +3900,44 @@
       <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="36">
+      <c r="A22" s="35">
         <v>20</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39">
+      <c r="A23" s="34">
         <v>21</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+      <c r="B23"/>
       <c r="E23" s="12"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="38">
+      <c r="A24" s="36">
         <v>22</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="39">
+      <c r="A25" s="34">
         <v>23</v>
       </c>
       <c r="B25"/>
@@ -4359,21 +3946,21 @@
       <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="34">
+      <c r="A26" s="33">
         <v>24</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="39">
+      <c r="A27" s="34">
         <v>25</v>
       </c>
       <c r="B27"/>
@@ -4382,21 +3969,21 @@
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="34">
+      <c r="A28" s="33">
         <v>26</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
     </row>
     <row r="29" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="39">
+      <c r="A29" s="34">
         <v>27</v>
       </c>
       <c r="B29"/>
@@ -4405,55 +3992,55 @@
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34">
+      <c r="A30" s="33">
         <v>28</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
     </row>
     <row r="31" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="40">
+      <c r="A31" s="37">
         <v>29</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27" t="s">
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H33" s="27" t="s">
+      <c r="H33" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="I33" s="27" t="s">
+      <c r="I33" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="J33" s="27" t="s">
+      <c r="J33" s="26" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4461,14 +4048,14 @@
       <c r="A34" s="1">
         <v>0</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="42"/>
+      <c r="C34" s="39"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="43" t="s">
+      <c r="G34" s="40" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="1">
@@ -4485,14 +4072,14 @@
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="42"/>
+      <c r="C35" s="39"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="25" t="s">
+      <c r="G35" s="24" t="s">
         <v>52</v>
       </c>
       <c r="H35" s="1">
@@ -4509,14 +4096,14 @@
       <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="42"/>
+      <c r="C36" s="39"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="25" t="s">
+      <c r="G36" s="24" t="s">
         <v>53</v>
       </c>
       <c r="H36" s="1">
@@ -4533,14 +4120,14 @@
       <c r="A37" s="1">
         <v>3</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="42"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="25" t="s">
+      <c r="G37" s="24" t="s">
         <v>54</v>
       </c>
       <c r="H37" s="1">
@@ -4557,14 +4144,14 @@
       <c r="A38" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="42"/>
+      <c r="C38" s="39"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="25" t="s">
+      <c r="G38" s="24" t="s">
         <v>55</v>
       </c>
       <c r="H38" s="1">
@@ -4584,7 +4171,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="25" t="s">
+      <c r="G39" s="24" t="s">
         <v>56</v>
       </c>
       <c r="H39" s="1">

</xml_diff>

<commit_message>
vault backup: 2025-12-16 20:27:25
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DEA29F-5C56-41AD-AA32-72C07BF886F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB8C548-4961-486B-B0E5-8EDA700813F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24504" yWindow="0" windowWidth="17868" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fighter A" sheetId="3" r:id="rId1"/>
-    <sheet name="Cleric A" sheetId="1" r:id="rId2"/>
-    <sheet name="Oggetti" sheetId="2" r:id="rId3"/>
+    <sheet name="Nano A" sheetId="6" r:id="rId1"/>
+    <sheet name="Ladro A" sheetId="5" r:id="rId2"/>
+    <sheet name="Magic A" sheetId="4" r:id="rId3"/>
+    <sheet name="Fighter A" sheetId="3" r:id="rId4"/>
+    <sheet name="Cleric A" sheetId="1" r:id="rId5"/>
+    <sheet name="Oggetti" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="212">
   <si>
     <t>Giocatore</t>
   </si>
@@ -506,6 +509,174 @@
   </si>
   <si>
     <t>Ritirata difensiva, mezzo movimento, no attacco</t>
+  </si>
+  <si>
+    <t>Juven Lionsbane</t>
+  </si>
+  <si>
+    <t>Mago</t>
+  </si>
+  <si>
+    <t>5°</t>
+  </si>
+  <si>
+    <t>Common, Orc, Ogre</t>
+  </si>
+  <si>
+    <t>Apre porte bloccate con 1 su 1d6</t>
+  </si>
+  <si>
+    <t>Bonus punti ferita aggiunti al totale</t>
+  </si>
+  <si>
+    <t>Legge e scrive più lingue</t>
+  </si>
+  <si>
+    <t>Reazioni PNG -1, massimo 3 seguaci, morale seguaci 6</t>
+  </si>
+  <si>
+    <t>38km</t>
+  </si>
+  <si>
+    <t>24mi</t>
+  </si>
+  <si>
+    <t>2/Bastone</t>
+  </si>
+  <si>
+    <t>1/Pugnali (2)</t>
+  </si>
+  <si>
+    <t>1/Libro Incantesimi</t>
+  </si>
+  <si>
+    <t>Bastone</t>
+  </si>
+  <si>
+    <t>1d4-1</t>
+  </si>
+  <si>
+    <t>10/20/30'</t>
+  </si>
+  <si>
+    <t>Palla di Fuoco 5d6 240</t>
+  </si>
+  <si>
+    <t>Dardo Incantato 2d6+2 150, Scudo CA2</t>
+  </si>
+  <si>
+    <t>Immagine Speculare 1d4 6T, Levitare 11T</t>
+  </si>
+  <si>
+    <t>Fragile Arcano Potente</t>
+  </si>
+  <si>
+    <t>Ladro</t>
+  </si>
+  <si>
+    <t>Cesaire Thorn</t>
+  </si>
+  <si>
+    <t>12mi</t>
+  </si>
+  <si>
+    <t>Common, Gnomesco</t>
+  </si>
+  <si>
+    <t>Spada</t>
+  </si>
+  <si>
+    <t>Arco Corto</t>
+  </si>
+  <si>
+    <t>50/100/150'</t>
+  </si>
+  <si>
+    <t>2/Armatura di cuoio +1</t>
+  </si>
+  <si>
+    <t>2/Arco Corto</t>
+  </si>
+  <si>
+    <t>1/Atrezzi da scasso</t>
+  </si>
+  <si>
+    <t>2/Spada</t>
+  </si>
+  <si>
+    <t>3/6 Ascoltare rumori</t>
+  </si>
+  <si>
+    <t>3/6 ascoltare attr. Porte</t>
+  </si>
+  <si>
+    <t>Scassinare</t>
+  </si>
+  <si>
+    <t>Borseggiare</t>
+  </si>
+  <si>
+    <t>Muoversi Silenziosamente</t>
+  </si>
+  <si>
+    <t>Scalare Parti Lisce</t>
+  </si>
+  <si>
+    <t>Nascondersi nelle Ombre</t>
+  </si>
+  <si>
+    <t>Trov./Rim. Trappole</t>
+  </si>
+  <si>
+    <t>Leg. Lingue non Magiche</t>
+  </si>
+  <si>
+    <t>Attacco alle Spalle +4 TxC, Danno x 2</t>
+  </si>
+  <si>
+    <t>Agile Furtivo Preciso</t>
+  </si>
+  <si>
+    <t>Seska Poluth</t>
+  </si>
+  <si>
+    <t>Nano</t>
+  </si>
+  <si>
+    <t>+7</t>
+  </si>
+  <si>
+    <t>Apre porte bloccate con 1-3 su 1d6</t>
+  </si>
+  <si>
+    <t>Legge e scrive nella lingua nativa</t>
+  </si>
+  <si>
+    <t>Bonus ai TS contro magia</t>
+  </si>
+  <si>
+    <t>Common, Nanco, Gnomesco, Koboldo,Goblin</t>
+  </si>
+  <si>
+    <t>Infravsione 60'/12q</t>
+  </si>
+  <si>
+    <t>1d8+1</t>
+  </si>
+  <si>
+    <t>50/100/150</t>
+  </si>
+  <si>
+    <t>1d4+1</t>
+  </si>
+  <si>
+    <t>1 mano  1d6+1</t>
+  </si>
+  <si>
+    <t>2/Ascia da Battaglia</t>
+  </si>
+  <si>
+    <t>2/Scudo</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1384,6 +1555,121 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1844,11 +2130,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D6BBBE-C9DF-4D21-98BF-29E96594E7D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06982626-440A-421A-816A-4B07BD0E71A6}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1866,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="82" t="s">
-        <v>133</v>
+        <v>198</v>
       </c>
       <c r="C1" s="82"/>
       <c r="D1" s="83"/>
@@ -1894,6 +2180,1125 @@
         <v>120</v>
       </c>
       <c r="B2" s="90" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="H2" s="93"/>
+      <c r="I2" s="100" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="124"/>
+      <c r="K2" s="125" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
+      <c r="N2" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="90"/>
+      <c r="P2" s="96"/>
+    </row>
+    <row r="3" spans="1:16" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="44"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="127"/>
+      <c r="O3" s="127"/>
+      <c r="P3" s="45"/>
+    </row>
+    <row r="4" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="129">
+        <v>2</v>
+      </c>
+      <c r="C4" s="130"/>
+      <c r="D4" s="131" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="130"/>
+      <c r="F4" s="132">
+        <v>22</v>
+      </c>
+      <c r="G4" s="133" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="134" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="130"/>
+      <c r="M4" s="135">
+        <v>0</v>
+      </c>
+      <c r="N4" s="130"/>
+      <c r="O4" s="131" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="98">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128" t="s">
+        <v>118</v>
+      </c>
+      <c r="K5" s="128"/>
+      <c r="L5" s="128"/>
+      <c r="M5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="53"/>
+    </row>
+    <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="80">
+        <v>13</v>
+      </c>
+      <c r="B6" s="134" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="136" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="132">
+        <v>1</v>
+      </c>
+      <c r="K6" s="132"/>
+      <c r="L6" s="128"/>
+      <c r="M6" s="137" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="137"/>
+      <c r="O6" s="137"/>
+      <c r="P6" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="80">
+        <v>10</v>
+      </c>
+      <c r="B7" s="134" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="136" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="136"/>
+      <c r="I7" s="136"/>
+      <c r="J7" s="132">
+        <v>0</v>
+      </c>
+      <c r="K7" s="132"/>
+      <c r="L7" s="128"/>
+      <c r="M7" s="137" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="137"/>
+      <c r="O7" s="137"/>
+      <c r="P7" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="80">
+        <v>16</v>
+      </c>
+      <c r="B8" s="134" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="136" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="136"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="136"/>
+      <c r="J8" s="132">
+        <v>2</v>
+      </c>
+      <c r="K8" s="132"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="137" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="137"/>
+      <c r="O8" s="137"/>
+      <c r="P8" s="54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="80">
+        <v>10</v>
+      </c>
+      <c r="B9" s="134" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="136" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="136"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="132">
+        <v>0</v>
+      </c>
+      <c r="K9" s="132"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="137" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="137"/>
+      <c r="O9" s="137"/>
+      <c r="P9" s="54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="80">
+        <v>13</v>
+      </c>
+      <c r="B10" s="134" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="136" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="136"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="136"/>
+      <c r="J10" s="132">
+        <v>1</v>
+      </c>
+      <c r="K10" s="132"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="137" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="137"/>
+      <c r="O10" s="137"/>
+      <c r="P10" s="54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="80">
+        <v>11</v>
+      </c>
+      <c r="B11" s="134" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="136" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="132">
+        <v>0</v>
+      </c>
+      <c r="K11" s="132"/>
+      <c r="L11" s="128"/>
+      <c r="M11" s="128"/>
+      <c r="N11" s="128"/>
+      <c r="O11" s="128"/>
+      <c r="P11" s="55"/>
+    </row>
+    <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="56"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="128"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
+      <c r="J12" s="128"/>
+      <c r="K12" s="128"/>
+      <c r="L12" s="128"/>
+      <c r="M12" s="128"/>
+      <c r="N12" s="128"/>
+      <c r="O12" s="128"/>
+      <c r="P12" s="55"/>
+    </row>
+    <row r="13" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="127"/>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="139" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="139" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="139" t="s">
+        <v>93</v>
+      </c>
+      <c r="L13" s="127"/>
+      <c r="M13" s="127"/>
+      <c r="N13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" s="5"/>
+      <c r="P13" s="59"/>
+    </row>
+    <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="111" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" s="140"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="138" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="138"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="141" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="142">
+        <v>20</v>
+      </c>
+      <c r="J14" s="130">
+        <f>K14*1.5</f>
+        <v>6</v>
+      </c>
+      <c r="K14" s="130">
+        <f>I14/5</f>
+        <v>4</v>
+      </c>
+      <c r="L14" s="127"/>
+      <c r="M14" s="127"/>
+      <c r="N14" s="127" t="s">
+        <v>80</v>
+      </c>
+      <c r="O14" s="127"/>
+      <c r="P14" s="45"/>
+    </row>
+    <row r="15" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="111"/>
+      <c r="B15" s="140"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="143"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="145" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="146">
+        <v>60</v>
+      </c>
+      <c r="J15" s="146">
+        <f>K15*1.5</f>
+        <v>18</v>
+      </c>
+      <c r="K15" s="146">
+        <f t="shared" ref="K15:K18" si="0">I15/5</f>
+        <v>12</v>
+      </c>
+      <c r="L15" s="127"/>
+      <c r="M15" s="127"/>
+      <c r="N15" s="127" t="s">
+        <v>167</v>
+      </c>
+      <c r="O15" s="127"/>
+      <c r="P15" s="45"/>
+    </row>
+    <row r="16" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="111"/>
+      <c r="B16" s="140"/>
+      <c r="C16" s="127"/>
+      <c r="D16" s="127"/>
+      <c r="E16" s="138" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="138"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="141" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" s="142">
+        <v>60</v>
+      </c>
+      <c r="J16" s="130">
+        <f>K16*1.5</f>
+        <v>18</v>
+      </c>
+      <c r="K16" s="130">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="127" t="s">
+        <v>184</v>
+      </c>
+      <c r="O16" s="127"/>
+      <c r="P16" s="45"/>
+    </row>
+    <row r="17" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="111"/>
+      <c r="B17" s="140"/>
+      <c r="C17" s="127"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="143"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="145" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="146">
+        <v>10</v>
+      </c>
+      <c r="J17" s="146">
+        <f>K17*1.5</f>
+        <v>3</v>
+      </c>
+      <c r="K17" s="146">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L17" s="127"/>
+      <c r="M17" s="127"/>
+      <c r="N17" s="127" t="s">
+        <v>83</v>
+      </c>
+      <c r="O17" s="127"/>
+      <c r="P17" s="45"/>
+    </row>
+    <row r="18" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44"/>
+      <c r="B18" s="127"/>
+      <c r="C18" s="127"/>
+      <c r="D18" s="127"/>
+      <c r="E18" s="138" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="138"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="141" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="142">
+        <v>10</v>
+      </c>
+      <c r="J18" s="130">
+        <f>K18*1.5</f>
+        <v>3</v>
+      </c>
+      <c r="K18" s="130">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L18" s="127"/>
+      <c r="M18" s="127"/>
+      <c r="N18" s="127" t="s">
+        <v>210</v>
+      </c>
+      <c r="O18" s="127"/>
+      <c r="P18" s="45"/>
+    </row>
+    <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="127"/>
+      <c r="D19" s="127"/>
+      <c r="E19" s="143" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="143"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="145" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" s="147" t="s">
+        <v>95</v>
+      </c>
+      <c r="J19" s="147" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" s="147"/>
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="127" t="s">
+        <v>211</v>
+      </c>
+      <c r="O19" s="127"/>
+      <c r="P19" s="45"/>
+    </row>
+    <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="67">
+        <v>0</v>
+      </c>
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="127"/>
+      <c r="K20" s="127"/>
+      <c r="L20" s="127"/>
+      <c r="M20" s="127"/>
+      <c r="N20" s="148" t="s">
+        <v>149</v>
+      </c>
+      <c r="O20" s="148"/>
+      <c r="P20" s="104"/>
+    </row>
+    <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="67">
+        <v>500</v>
+      </c>
+      <c r="C21" s="127"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="149" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="127"/>
+      <c r="G21" s="127"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="127"/>
+      <c r="J21" s="127"/>
+      <c r="K21" s="127"/>
+      <c r="L21" s="127"/>
+      <c r="M21" s="127"/>
+      <c r="N21" s="127"/>
+      <c r="O21" s="150" t="s">
+        <v>48</v>
+      </c>
+      <c r="P21" s="69">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="67">
+        <v>0</v>
+      </c>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="128" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="128"/>
+      <c r="J22" s="128"/>
+      <c r="K22" s="128"/>
+      <c r="L22" s="128"/>
+      <c r="M22" s="128"/>
+      <c r="N22" s="127"/>
+      <c r="O22" s="150" t="s">
+        <v>41</v>
+      </c>
+      <c r="P22" s="69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="67">
+        <v>0</v>
+      </c>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
+      <c r="J23" s="128"/>
+      <c r="K23" s="128"/>
+      <c r="L23" s="128"/>
+      <c r="M23" s="138"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="128"/>
+      <c r="P23" s="55"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="128"/>
+      <c r="L24" s="128"/>
+      <c r="M24" s="138"/>
+      <c r="N24" s="138"/>
+      <c r="O24" s="128"/>
+      <c r="P24" s="55"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="56"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="128"/>
+      <c r="L25" s="128"/>
+      <c r="M25" s="128"/>
+      <c r="N25" s="128"/>
+      <c r="O25" s="128"/>
+      <c r="P25" s="55"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="56"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="128"/>
+      <c r="L26" s="128"/>
+      <c r="M26" s="128"/>
+      <c r="N26" s="128"/>
+      <c r="O26" s="128"/>
+      <c r="P26" s="55"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="115" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="152"/>
+      <c r="C27" s="152" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="128"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="128"/>
+      <c r="N27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="6"/>
+      <c r="P27" s="53"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="118" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="153"/>
+      <c r="C28" s="154">
+        <v>2</v>
+      </c>
+      <c r="D28" s="128"/>
+      <c r="E28" s="128"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="128"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="128"/>
+      <c r="J28" s="128"/>
+      <c r="K28" s="128"/>
+      <c r="L28" s="128"/>
+      <c r="M28" s="128"/>
+      <c r="N28" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="O28" s="128"/>
+      <c r="P28" s="55"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="118" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="153"/>
+      <c r="C29" s="153">
+        <v>3</v>
+      </c>
+      <c r="D29" s="128"/>
+      <c r="E29" s="128"/>
+      <c r="F29" s="128"/>
+      <c r="G29" s="128"/>
+      <c r="H29" s="128"/>
+      <c r="I29" s="128"/>
+      <c r="J29" s="128"/>
+      <c r="K29" s="128"/>
+      <c r="L29" s="128"/>
+      <c r="M29" s="128"/>
+      <c r="N29" s="128" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29" s="128"/>
+      <c r="P29" s="55"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="118" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="153"/>
+      <c r="C30" s="153">
+        <v>3</v>
+      </c>
+      <c r="D30" s="128"/>
+      <c r="E30" s="128"/>
+      <c r="F30" s="128"/>
+      <c r="G30" s="128"/>
+      <c r="H30" s="128"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="128"/>
+      <c r="K30" s="128"/>
+      <c r="L30" s="128"/>
+      <c r="M30" s="128"/>
+      <c r="N30" s="128" t="s">
+        <v>78</v>
+      </c>
+      <c r="O30" s="128"/>
+      <c r="P30" s="55"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="118" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="153"/>
+      <c r="C31" s="153">
+        <v>3</v>
+      </c>
+      <c r="D31" s="128"/>
+      <c r="E31" s="128"/>
+      <c r="F31" s="128"/>
+      <c r="G31" s="128"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="128"/>
+      <c r="J31" s="128"/>
+      <c r="K31" s="128"/>
+      <c r="L31" s="128"/>
+      <c r="M31" s="128"/>
+      <c r="N31" s="128" t="s">
+        <v>205</v>
+      </c>
+      <c r="O31" s="128"/>
+      <c r="P31" s="55"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="56"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="128"/>
+      <c r="H32" s="128"/>
+      <c r="I32" s="128"/>
+      <c r="J32" s="128"/>
+      <c r="K32" s="128"/>
+      <c r="L32" s="128"/>
+      <c r="M32" s="128"/>
+      <c r="N32" s="128"/>
+      <c r="O32" s="128"/>
+      <c r="P32" s="55"/>
+    </row>
+    <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="9">
+        <v>8</v>
+      </c>
+      <c r="E33" s="10">
+        <f>D33-1</f>
+        <v>7</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" ref="F33:L33" si="1">E33-1</f>
+        <v>6</v>
+      </c>
+      <c r="G33" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J33" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K33" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L33" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="N33" s="105"/>
+      <c r="O33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" s="53"/>
+    </row>
+    <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
+      <c r="A34" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="130" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="155">
+        <v>7</v>
+      </c>
+      <c r="D34" s="156">
+        <f>C34+1</f>
+        <v>8</v>
+      </c>
+      <c r="E34" s="155">
+        <f t="shared" ref="E34:L34" si="2">D34+1</f>
+        <v>9</v>
+      </c>
+      <c r="F34" s="156">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G34" s="155">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="H34" s="156">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="I34" s="155">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="J34" s="156">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="K34" s="155">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="L34" s="156">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M34" s="106" t="s">
+        <v>206</v>
+      </c>
+      <c r="N34" s="106"/>
+      <c r="O34" s="128" t="s">
+        <v>209</v>
+      </c>
+      <c r="P34" s="55"/>
+    </row>
+    <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
+      <c r="A35" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="130" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="155">
+        <v>7</v>
+      </c>
+      <c r="D35" s="156">
+        <f t="shared" ref="D35:L36" si="3">C35+1</f>
+        <v>8</v>
+      </c>
+      <c r="E35" s="155">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="F35" s="156">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G35" s="155">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="H35" s="156">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="I35" s="155">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="J35" s="156">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="K35" s="155">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="L35" s="156">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="M35" s="157" t="s">
+        <v>208</v>
+      </c>
+      <c r="N35" s="157"/>
+      <c r="O35" s="127" t="s">
+        <v>147</v>
+      </c>
+      <c r="P35" s="55"/>
+    </row>
+    <row r="36" spans="1:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="74" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="75" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" s="76">
+        <v>8</v>
+      </c>
+      <c r="D36" s="77">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="E36" s="76">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F36" s="77">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G36" s="76">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="H36" s="77">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="I36" s="76">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J36" s="77">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="K36" s="76">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="L36" s="77">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="M36" s="108" t="s">
+        <v>28</v>
+      </c>
+      <c r="N36" s="108"/>
+      <c r="O36" s="78" t="s">
+        <v>148</v>
+      </c>
+      <c r="P36" s="79"/>
+      <c r="AA36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="M8:O8"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E67570B-E252-4754-963B-16F0C4F39BE1}">
+  <dimension ref="A1:AA36"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="2" customWidth="1"/>
+    <col min="3" max="12" width="4.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="4.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="101" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="82"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="82"/>
+      <c r="P1" s="88"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="90" t="s">
         <v>100</v>
       </c>
       <c r="C2" s="90"/>
@@ -1903,7 +3308,7 @@
       </c>
       <c r="F2" s="93"/>
       <c r="G2" s="93" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="H2" s="93"/>
       <c r="I2" s="100" t="s">
@@ -1942,6 +3347,1808 @@
         <v>8</v>
       </c>
       <c r="B4" s="47">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="49">
+        <v>20</v>
+      </c>
+      <c r="G4" s="102" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="51">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="98">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="J5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="53"/>
+    </row>
+    <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="80">
+        <v>9</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="109" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="49">
+        <v>0</v>
+      </c>
+      <c r="K6" s="49"/>
+      <c r="M6" s="110" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="54">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="80">
+        <v>16</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="109" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="49">
+        <v>2</v>
+      </c>
+      <c r="K7" s="49"/>
+      <c r="M7" s="110" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="110"/>
+      <c r="O7" s="110"/>
+      <c r="P7" s="54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="80">
+        <v>13</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="109" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="49">
+        <v>1</v>
+      </c>
+      <c r="K8" s="49"/>
+      <c r="M8" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="54">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="80">
+        <v>14</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="109" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="49">
+        <v>1</v>
+      </c>
+      <c r="K9" s="49"/>
+      <c r="M9" s="110" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="80">
+        <v>6</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="109" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="49">
+        <v>-1</v>
+      </c>
+      <c r="K10" s="49"/>
+      <c r="M10" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="110"/>
+      <c r="O10" s="110"/>
+      <c r="P10" s="54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="80">
+        <v>10</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="109" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="49">
+        <v>0</v>
+      </c>
+      <c r="K11" s="49"/>
+      <c r="P11" s="55"/>
+    </row>
+    <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="56"/>
+      <c r="P12" s="55"/>
+    </row>
+    <row r="13" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="41"/>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" s="5"/>
+      <c r="P13" s="59"/>
+    </row>
+    <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="112"/>
+      <c r="E14" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="41"/>
+      <c r="H14" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="61">
+        <v>40</v>
+      </c>
+      <c r="J14" s="1">
+        <f>K14*1.5</f>
+        <v>12</v>
+      </c>
+      <c r="K14" s="1">
+        <f>I14/5</f>
+        <v>8</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P14" s="45"/>
+    </row>
+    <row r="15" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="111"/>
+      <c r="B15" s="112"/>
+      <c r="E15" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="65">
+        <f>I14*3</f>
+        <v>120</v>
+      </c>
+      <c r="J15" s="65">
+        <f>K15*1.5</f>
+        <v>36</v>
+      </c>
+      <c r="K15" s="65">
+        <f t="shared" ref="K15:K18" si="0">I15/5</f>
+        <v>24</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P15" s="45"/>
+    </row>
+    <row r="16" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112"/>
+      <c r="E16" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="H16" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" s="61">
+        <f>I14*3</f>
+        <v>120</v>
+      </c>
+      <c r="J16" s="1">
+        <f>K16*1.5</f>
+        <v>36</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="P16" s="45"/>
+    </row>
+    <row r="17" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="111"/>
+      <c r="B17" s="112"/>
+      <c r="E17" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="65">
+        <f>I14/2</f>
+        <v>20</v>
+      </c>
+      <c r="J17" s="65">
+        <f>K17*1.5</f>
+        <v>6</v>
+      </c>
+      <c r="K17" s="65">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P17" s="45"/>
+    </row>
+    <row r="18" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44"/>
+      <c r="E18" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="41"/>
+      <c r="H18" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="61">
+        <f>I14/2</f>
+        <v>20</v>
+      </c>
+      <c r="J18" s="1">
+        <f>K18*1.5</f>
+        <v>6</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="P18" s="45"/>
+    </row>
+    <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="E19" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="K19" s="66"/>
+      <c r="N19" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="P19" s="45"/>
+    </row>
+    <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="67">
+        <v>0</v>
+      </c>
+      <c r="N20" s="103" t="s">
+        <v>149</v>
+      </c>
+      <c r="O20" s="103"/>
+      <c r="P20" s="104"/>
+    </row>
+    <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="67">
+        <v>500</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="P21" s="69">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="67">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="P22" s="69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="67">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M23" s="41"/>
+      <c r="N23" s="42"/>
+      <c r="P23" s="55"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56"/>
+      <c r="E24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="P24" s="55"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="121" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="123">
+        <v>0.45</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="P25" s="55"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="122" t="s">
+        <v>194</v>
+      </c>
+      <c r="C26" s="123">
+        <v>0.4</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P26" s="55"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="118" t="s">
+        <v>190</v>
+      </c>
+      <c r="B27" s="114"/>
+      <c r="C27" s="123">
+        <v>0.45</v>
+      </c>
+      <c r="E27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="N27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="6"/>
+      <c r="P27" s="53"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="116" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="117"/>
+      <c r="C28" s="123">
+        <v>0.45</v>
+      </c>
+      <c r="E28" s="120" t="s">
+        <v>196</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="P28" s="55"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="116" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" s="117"/>
+      <c r="C29" s="123">
+        <v>0.92</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="P29" s="55"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="118" t="s">
+        <v>193</v>
+      </c>
+      <c r="B30" s="117"/>
+      <c r="C30" s="123">
+        <v>0.36</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="P30" s="55"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="118" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" s="117"/>
+      <c r="C31" s="123">
+        <v>0.8</v>
+      </c>
+      <c r="P31" s="55"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="56"/>
+      <c r="P32" s="55"/>
+    </row>
+    <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="9">
+        <v>8</v>
+      </c>
+      <c r="E33" s="10">
+        <f>D33-1</f>
+        <v>7</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" ref="F33:L33" si="1">E33-1</f>
+        <v>6</v>
+      </c>
+      <c r="G33" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J33" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K33" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L33" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="N33" s="105"/>
+      <c r="O33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" s="53"/>
+    </row>
+    <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
+      <c r="A34" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="72">
+        <v>8</v>
+      </c>
+      <c r="D34" s="73">
+        <f>C34+1</f>
+        <v>9</v>
+      </c>
+      <c r="E34" s="72">
+        <f t="shared" ref="E34:L34" si="2">D34+1</f>
+        <v>10</v>
+      </c>
+      <c r="F34" s="73">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="G34" s="72">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H34" s="73">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="I34" s="72">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="J34" s="73">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="K34" s="72">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="L34" s="73">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="M34" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="N34" s="106"/>
+      <c r="P34" s="55"/>
+    </row>
+    <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
+      <c r="A35" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="72">
+        <v>8</v>
+      </c>
+      <c r="D35" s="73">
+        <f t="shared" ref="D35:L36" si="3">C35+1</f>
+        <v>9</v>
+      </c>
+      <c r="E35" s="72">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F35" s="73">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G35" s="72">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="H35" s="73">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="I35" s="72">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J35" s="73">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="K35" s="72">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="L35" s="73">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="M35" s="107" t="s">
+        <v>110</v>
+      </c>
+      <c r="N35" s="107"/>
+      <c r="O35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="P35" s="55"/>
+    </row>
+    <row r="36" spans="1:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="74" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="75" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="76">
+        <v>6</v>
+      </c>
+      <c r="D36" s="77">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E36" s="76">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="F36" s="77">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G36" s="76">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="H36" s="77">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="I36" s="76">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="J36" s="77">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="K36" s="76">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="L36" s="77">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="M36" s="108" t="s">
+        <v>28</v>
+      </c>
+      <c r="N36" s="108"/>
+      <c r="O36" s="78" t="s">
+        <v>148</v>
+      </c>
+      <c r="P36" s="79"/>
+      <c r="AA36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="M8:O8"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23066C9D-052A-4A0F-9F62-A1EE62475AEE}">
+  <dimension ref="A1:AA36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="2" customWidth="1"/>
+    <col min="3" max="12" width="4.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="4.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="82"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="82"/>
+      <c r="P1" s="88"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="93"/>
+      <c r="I2" s="100" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="91"/>
+      <c r="K2" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="90"/>
+      <c r="P2" s="96"/>
+    </row>
+    <row r="3" spans="1:16" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="44"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="45"/>
+    </row>
+    <row r="4" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="47">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="49">
+        <v>18</v>
+      </c>
+      <c r="G4" s="49">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="51">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="98">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="J5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="53"/>
+    </row>
+    <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="80">
+        <v>8</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="109" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="49">
+        <v>-1</v>
+      </c>
+      <c r="K6" s="49"/>
+      <c r="M6" s="110" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="80">
+        <v>10</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="49">
+        <v>0</v>
+      </c>
+      <c r="K7" s="49"/>
+      <c r="M7" s="110" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="110"/>
+      <c r="O7" s="110"/>
+      <c r="P7" s="54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="80">
+        <v>13</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="109" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="49">
+        <v>1</v>
+      </c>
+      <c r="K8" s="49"/>
+      <c r="M8" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="80">
+        <v>16</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="109" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="49">
+        <v>2</v>
+      </c>
+      <c r="K9" s="49"/>
+      <c r="M9" s="110" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="80">
+        <v>9</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="49">
+        <v>0</v>
+      </c>
+      <c r="K10" s="49"/>
+      <c r="M10" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="110"/>
+      <c r="O10" s="110"/>
+      <c r="P10" s="54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="80">
+        <v>8</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="109" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="49">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="49"/>
+      <c r="P11" s="55"/>
+    </row>
+    <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="56"/>
+      <c r="P12" s="55"/>
+    </row>
+    <row r="13" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="41"/>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" s="5"/>
+      <c r="P13" s="59"/>
+    </row>
+    <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="111" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="112"/>
+      <c r="E14" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="41"/>
+      <c r="H14" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="61">
+        <v>40</v>
+      </c>
+      <c r="J14" s="1">
+        <f>K14*1.5</f>
+        <v>12</v>
+      </c>
+      <c r="K14" s="1">
+        <f>I14/5</f>
+        <v>8</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="P14" s="45"/>
+    </row>
+    <row r="15" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="111"/>
+      <c r="B15" s="112"/>
+      <c r="E15" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="65">
+        <f>I14*3</f>
+        <v>120</v>
+      </c>
+      <c r="J15" s="65">
+        <f>K15*1.5</f>
+        <v>36</v>
+      </c>
+      <c r="K15" s="65">
+        <f t="shared" ref="K15:K18" si="0">I15/5</f>
+        <v>24</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P15" s="45"/>
+    </row>
+    <row r="16" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112"/>
+      <c r="E16" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="H16" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" s="61">
+        <f>I14*3</f>
+        <v>120</v>
+      </c>
+      <c r="J16" s="1">
+        <f>K16*1.5</f>
+        <v>36</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P16" s="45"/>
+    </row>
+    <row r="17" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="111"/>
+      <c r="B17" s="112"/>
+      <c r="E17" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="65">
+        <f>I14/2</f>
+        <v>20</v>
+      </c>
+      <c r="J17" s="65">
+        <f>K17*1.5</f>
+        <v>6</v>
+      </c>
+      <c r="K17" s="65">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="P17" s="45"/>
+    </row>
+    <row r="18" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44"/>
+      <c r="E18" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="41"/>
+      <c r="H18" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="61">
+        <f>I14/2</f>
+        <v>20</v>
+      </c>
+      <c r="J18" s="1">
+        <f>K18*1.5</f>
+        <v>6</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P18" s="45"/>
+    </row>
+    <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="E19" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="K19" s="66"/>
+      <c r="P19" s="45"/>
+    </row>
+    <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="67">
+        <v>0</v>
+      </c>
+      <c r="N20" s="103"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="104"/>
+    </row>
+    <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="67">
+        <v>500</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="P21" s="69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="67">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="P22" s="69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="67">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M23" s="41"/>
+      <c r="N23" s="42"/>
+      <c r="P23" s="55"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56"/>
+      <c r="E24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="P24" s="55"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="56"/>
+      <c r="E25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="P25" s="55"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="56"/>
+      <c r="P26" s="55"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="N27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="6"/>
+      <c r="P27" s="53"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="P28" s="55"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P29" s="55"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P30" s="55"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="119"/>
+      <c r="P31" s="55"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="56"/>
+      <c r="P32" s="55"/>
+    </row>
+    <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="9">
+        <v>8</v>
+      </c>
+      <c r="E33" s="10">
+        <f>D33-1</f>
+        <v>7</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" ref="F33:L33" si="1">E33-1</f>
+        <v>6</v>
+      </c>
+      <c r="G33" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J33" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K33" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L33" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="N33" s="105"/>
+      <c r="O33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" s="53"/>
+    </row>
+    <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
+      <c r="A34" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="72">
+        <v>11</v>
+      </c>
+      <c r="D34" s="73">
+        <f>C34+1</f>
+        <v>12</v>
+      </c>
+      <c r="E34" s="72">
+        <f t="shared" ref="E34:L34" si="2">D34+1</f>
+        <v>13</v>
+      </c>
+      <c r="F34" s="73">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G34" s="72">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="H34" s="73">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="I34" s="72">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="J34" s="73">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="K34" s="72">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="L34" s="73">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M34" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="N34" s="106"/>
+      <c r="P34" s="55"/>
+    </row>
+    <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
+      <c r="A35" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="72">
+        <v>11</v>
+      </c>
+      <c r="D35" s="73">
+        <f t="shared" ref="D35:L36" si="3">C35+1</f>
+        <v>12</v>
+      </c>
+      <c r="E35" s="72">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="F35" s="73">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="G35" s="72">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="H35" s="73">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I35" s="72">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="J35" s="73">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="K35" s="72">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="L35" s="73">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="M35" s="107" t="s">
+        <v>170</v>
+      </c>
+      <c r="N35" s="107"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="55"/>
+    </row>
+    <row r="36" spans="1:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="76">
+        <v>10</v>
+      </c>
+      <c r="D36" s="77">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="E36" s="76">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="F36" s="77">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="G36" s="76">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="H36" s="77">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="I36" s="76">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="J36" s="77">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="K36" s="76">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="L36" s="77">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="M36" s="108" t="s">
+        <v>110</v>
+      </c>
+      <c r="N36" s="108"/>
+      <c r="O36" s="78"/>
+      <c r="P36" s="79"/>
+      <c r="AA36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="M8:O8"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D6BBBE-C9DF-4D21-98BF-29E96594E7D0}">
+  <dimension ref="A1:AA36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="2" customWidth="1"/>
+    <col min="3" max="12" width="4.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="4.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="101" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="82"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="82"/>
+      <c r="P1" s="88"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="93"/>
+      <c r="I2" s="100" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="91"/>
+      <c r="K2" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="90"/>
+      <c r="P2" s="96"/>
+    </row>
+    <row r="3" spans="1:16" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="44"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="45"/>
+    </row>
+    <row r="4" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="47">
         <v>0</v>
       </c>
       <c r="C4" s="1"/>
@@ -2202,6 +5409,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="1">
+        <f>K14*1.5</f>
         <v>6</v>
       </c>
       <c r="K14" s="1">
@@ -2228,6 +5436,7 @@
         <v>60</v>
       </c>
       <c r="J15" s="65">
+        <f>K15*1.5</f>
         <v>18</v>
       </c>
       <c r="K15" s="65">
@@ -2253,6 +5462,7 @@
         <v>60</v>
       </c>
       <c r="J16" s="1">
+        <f>K16*1.5</f>
         <v>18</v>
       </c>
       <c r="K16" s="1">
@@ -2279,6 +5489,7 @@
         <v>10</v>
       </c>
       <c r="J17" s="65">
+        <f>K17*1.5</f>
         <v>3</v>
       </c>
       <c r="K17" s="65">
@@ -2303,6 +5514,7 @@
         <v>10</v>
       </c>
       <c r="J18" s="1">
+        <f>K18*1.5</f>
         <v>3</v>
       </c>
       <c r="K18" s="1">
@@ -2738,12 +5950,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263CECC3-3302-44DA-8376-3DD3643BBD45}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3097,6 +6309,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="1">
+        <f>K14*1.5</f>
         <v>6</v>
       </c>
       <c r="K14" s="1">
@@ -3123,6 +6336,7 @@
         <v>60</v>
       </c>
       <c r="J15" s="65">
+        <f>K15*1.5</f>
         <v>18</v>
       </c>
       <c r="K15" s="65">
@@ -3148,6 +6362,7 @@
         <v>60</v>
       </c>
       <c r="J16" s="1">
+        <f>K16*1.5</f>
         <v>18</v>
       </c>
       <c r="K16" s="1">
@@ -3174,6 +6389,7 @@
         <v>10</v>
       </c>
       <c r="J17" s="65">
+        <f>K17*1.5</f>
         <v>3</v>
       </c>
       <c r="K17" s="65">
@@ -3198,6 +6414,7 @@
         <v>10</v>
       </c>
       <c r="J18" s="1">
+        <f>K18*1.5</f>
         <v>3</v>
       </c>
       <c r="K18" s="1">
@@ -3223,7 +6440,7 @@
         <v>98</v>
       </c>
       <c r="I19" s="66" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="J19" s="66" t="s">
         <v>94</v>
@@ -3639,7 +6856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7F733B-4F29-4CC7-8875-78DA591CD6C7}">
   <dimension ref="A1:J76"/>
   <sheetViews>

</xml_diff>

<commit_message>
vault backup: 2025-12-16 22:24:58
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB8C548-4961-486B-B0E5-8EDA700813F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5217A6D9-5C94-4D62-885A-B5AA8A96D60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24504" yWindow="0" windowWidth="17868" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nano A" sheetId="6" r:id="rId1"/>
-    <sheet name="Ladro A" sheetId="5" r:id="rId2"/>
-    <sheet name="Magic A" sheetId="4" r:id="rId3"/>
-    <sheet name="Fighter A" sheetId="3" r:id="rId4"/>
-    <sheet name="Cleric A" sheetId="1" r:id="rId5"/>
-    <sheet name="Oggetti" sheetId="2" r:id="rId6"/>
+    <sheet name="Elfo A" sheetId="7" r:id="rId1"/>
+    <sheet name="Nano A" sheetId="6" r:id="rId2"/>
+    <sheet name="Ladro A" sheetId="5" r:id="rId3"/>
+    <sheet name="Magic A" sheetId="4" r:id="rId4"/>
+    <sheet name="Fighter A" sheetId="3" r:id="rId5"/>
+    <sheet name="Cleric A" sheetId="1" r:id="rId6"/>
+    <sheet name="Oggetti" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="223">
   <si>
     <t>Giocatore</t>
   </si>
@@ -677,6 +678,39 @@
   </si>
   <si>
     <t>2/Scudo</t>
+  </si>
+  <si>
+    <t>Nano Corazzato Resistente</t>
+  </si>
+  <si>
+    <t>Conno Darhov</t>
+  </si>
+  <si>
+    <t>Elfo</t>
+  </si>
+  <si>
+    <t>33,650</t>
+  </si>
+  <si>
+    <t>Elfico, Comune, Orchesco, Hobgoblin, Gnoll, Draconico, Pixie</t>
+  </si>
+  <si>
+    <t>2/6 trovare porte segrete</t>
+  </si>
+  <si>
+    <t>Immune paralisi Ghoul</t>
+  </si>
+  <si>
+    <t>1d8+2</t>
+  </si>
+  <si>
+    <t>Fulmine 5d6 60'x5'</t>
+  </si>
+  <si>
+    <t>Dardo Incantato 2d6+2 150' x 2</t>
+  </si>
+  <si>
+    <t>Immagine Speculare 1d4 6T, Scassinare 60'</t>
   </si>
 </sst>
 </file>
@@ -2130,11 +2164,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06982626-440A-421A-816A-4B07BD0E71A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF42BED5-6492-4A4B-BB83-28F0C7345C12}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2152,14 +2186,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="82" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="C1" s="82"/>
       <c r="D1" s="83"/>
       <c r="E1" s="99"/>
       <c r="F1" s="84"/>
       <c r="G1" s="101" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="H1" s="82"/>
       <c r="I1" s="84"/>
@@ -2170,7 +2204,7 @@
       <c r="L1" s="83"/>
       <c r="M1" s="83"/>
       <c r="N1" s="87" t="s">
-        <v>121</v>
+        <v>215</v>
       </c>
       <c r="O1" s="82"/>
       <c r="P1" s="88"/>
@@ -2180,27 +2214,27 @@
         <v>120</v>
       </c>
       <c r="B2" s="90" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="C2" s="90"/>
-      <c r="D2" s="124"/>
+      <c r="D2" s="91"/>
       <c r="E2" s="92" t="s">
         <v>33</v>
       </c>
       <c r="F2" s="93"/>
       <c r="G2" s="93" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="H2" s="93"/>
       <c r="I2" s="100" t="s">
         <v>158</v>
       </c>
-      <c r="J2" s="124"/>
-      <c r="K2" s="125" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
       <c r="N2" s="90" t="s">
         <v>72</v>
       </c>
@@ -2209,56 +2243,54 @@
     </row>
     <row r="3" spans="1:16" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
-      <c r="O3" s="127"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
       <c r="P3" s="45"/>
     </row>
     <row r="4" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="129">
-        <v>2</v>
-      </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="131" t="s">
+      <c r="B4" s="47">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="132">
-        <v>22</v>
-      </c>
-      <c r="G4" s="133" t="s">
-        <v>200</v>
-      </c>
-      <c r="H4" s="130"/>
-      <c r="I4" s="130"/>
-      <c r="J4" s="130"/>
-      <c r="K4" s="134" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="49">
+        <v>24</v>
+      </c>
+      <c r="G4" s="102" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="L4" s="130"/>
-      <c r="M4" s="135">
+      <c r="L4" s="1"/>
+      <c r="M4" s="51">
         <v>0</v>
       </c>
-      <c r="N4" s="130"/>
-      <c r="O4" s="131" t="s">
+      <c r="N4" s="1"/>
+      <c r="O4" s="48" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="98">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2266,18 +2298,9 @@
         <v>29</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128" t="s">
+      <c r="J5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K5" s="128"/>
-      <c r="L5" s="128"/>
       <c r="M5" s="7" t="s">
         <v>10</v>
       </c>
@@ -2287,196 +2310,173 @@
     </row>
     <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="80">
-        <v>13</v>
-      </c>
-      <c r="B6" s="134" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="136" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="132">
-        <v>1</v>
-      </c>
-      <c r="K6" s="132"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="137" t="s">
+      <c r="C6" s="109" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="49">
+        <v>2</v>
+      </c>
+      <c r="K6" s="49"/>
+      <c r="M6" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="N6" s="137"/>
-      <c r="O6" s="137"/>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
       <c r="P6" s="54">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="80">
-        <v>10</v>
-      </c>
-      <c r="B7" s="134" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="136" t="s">
+      <c r="C7" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="132">
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="49">
         <v>0</v>
       </c>
-      <c r="K7" s="132"/>
-      <c r="L7" s="128"/>
-      <c r="M7" s="137" t="s">
+      <c r="K7" s="49"/>
+      <c r="M7" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="137"/>
-      <c r="O7" s="137"/>
+      <c r="N7" s="110"/>
+      <c r="O7" s="110"/>
       <c r="P7" s="54">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="80">
-        <v>16</v>
-      </c>
-      <c r="B8" s="134" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="136" t="s">
+      <c r="C8" s="109" t="s">
         <v>161</v>
       </c>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="132">
-        <v>2</v>
-      </c>
-      <c r="K8" s="132"/>
-      <c r="L8" s="128"/>
-      <c r="M8" s="137" t="s">
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="49">
+        <v>1</v>
+      </c>
+      <c r="K8" s="49"/>
+      <c r="M8" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="137"/>
-      <c r="O8" s="137"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
       <c r="P8" s="54">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="80">
-        <v>10</v>
-      </c>
-      <c r="B9" s="134" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="136" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
-      <c r="G9" s="136"/>
-      <c r="H9" s="136"/>
-      <c r="I9" s="136"/>
-      <c r="J9" s="132">
-        <v>0</v>
-      </c>
-      <c r="K9" s="132"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="137" t="s">
+      <c r="C9" s="109" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="49">
+        <v>2</v>
+      </c>
+      <c r="K9" s="49"/>
+      <c r="M9" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="137"/>
-      <c r="O9" s="137"/>
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
       <c r="P9" s="54">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="80">
+        <v>11</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="49">
+        <v>0</v>
+      </c>
+      <c r="K10" s="49"/>
+      <c r="M10" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="134" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="136" t="s">
-        <v>203</v>
-      </c>
-      <c r="D10" s="136"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="136"/>
-      <c r="I10" s="136"/>
-      <c r="J10" s="132">
-        <v>1</v>
-      </c>
-      <c r="K10" s="132"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="137" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" s="137"/>
-      <c r="O10" s="137"/>
+      <c r="N10" s="110"/>
+      <c r="O10" s="110"/>
       <c r="P10" s="54">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="80">
-        <v>11</v>
-      </c>
-      <c r="B11" s="134" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="136" t="s">
+      <c r="C11" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="136"/>
-      <c r="E11" s="136"/>
-      <c r="F11" s="136"/>
-      <c r="G11" s="136"/>
-      <c r="H11" s="136"/>
-      <c r="I11" s="136"/>
-      <c r="J11" s="132">
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="49">
         <v>0</v>
       </c>
-      <c r="K11" s="132"/>
-      <c r="L11" s="128"/>
-      <c r="M11" s="128"/>
-      <c r="N11" s="128"/>
-      <c r="O11" s="128"/>
+      <c r="K11" s="49"/>
       <c r="P11" s="55"/>
     </row>
     <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="56"/>
-      <c r="B12" s="128"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
-      <c r="I12" s="128"/>
-      <c r="J12" s="128"/>
-      <c r="K12" s="128"/>
-      <c r="L12" s="128"/>
-      <c r="M12" s="128"/>
-      <c r="N12" s="128"/>
-      <c r="O12" s="128"/>
       <c r="P12" s="55"/>
     </row>
     <row r="13" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2484,25 +2484,22 @@
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="127"/>
+      <c r="C13" s="41"/>
       <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="138"/>
-      <c r="I13" s="139" t="s">
+      <c r="H13" s="41"/>
+      <c r="I13" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="139" t="s">
+      <c r="J13" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="139" t="s">
+      <c r="K13" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="127"/>
-      <c r="M13" s="127"/>
       <c r="N13" s="4" t="s">
         <v>79</v>
       </c>
@@ -2511,164 +2508,136 @@
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="111" t="s">
-        <v>204</v>
-      </c>
-      <c r="B14" s="140"/>
-      <c r="C14" s="127"/>
-      <c r="D14" s="127"/>
-      <c r="E14" s="138" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="112"/>
+      <c r="E14" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="138"/>
-      <c r="G14" s="127"/>
-      <c r="H14" s="141" t="s">
+      <c r="F14" s="41"/>
+      <c r="H14" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="142">
+      <c r="I14" s="61">
         <v>20</v>
       </c>
-      <c r="J14" s="130">
+      <c r="J14" s="1">
         <f>K14*1.5</f>
         <v>6</v>
       </c>
-      <c r="K14" s="130">
+      <c r="K14" s="1">
         <f>I14/5</f>
         <v>4</v>
       </c>
-      <c r="L14" s="127"/>
-      <c r="M14" s="127"/>
-      <c r="N14" s="127" t="s">
-        <v>80</v>
-      </c>
-      <c r="O14" s="127"/>
+      <c r="N14" s="3" t="s">
+        <v>166</v>
+      </c>
       <c r="P14" s="45"/>
     </row>
     <row r="15" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="111"/>
-      <c r="B15" s="140"/>
-      <c r="C15" s="127"/>
-      <c r="D15" s="127"/>
-      <c r="E15" s="143" t="s">
+      <c r="B15" s="112"/>
+      <c r="E15" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="143"/>
-      <c r="G15" s="144"/>
-      <c r="H15" s="145" t="s">
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="146">
+      <c r="I15" s="65">
+        <f>I14*3</f>
         <v>60</v>
       </c>
-      <c r="J15" s="146">
+      <c r="J15" s="65">
         <f>K15*1.5</f>
         <v>18</v>
       </c>
-      <c r="K15" s="146">
+      <c r="K15" s="65">
         <f t="shared" ref="K15:K18" si="0">I15/5</f>
         <v>12</v>
       </c>
-      <c r="L15" s="127"/>
-      <c r="M15" s="127"/>
-      <c r="N15" s="127" t="s">
+      <c r="N15" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="O15" s="127"/>
       <c r="P15" s="45"/>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="111"/>
-      <c r="B16" s="140"/>
-      <c r="C16" s="127"/>
-      <c r="D16" s="127"/>
-      <c r="E16" s="138" t="s">
+      <c r="B16" s="112"/>
+      <c r="E16" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="138"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="141" t="s">
+      <c r="F16" s="41"/>
+      <c r="H16" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I16" s="142">
+      <c r="I16" s="61">
+        <f>I14*3</f>
         <v>60</v>
       </c>
-      <c r="J16" s="130">
+      <c r="J16" s="1">
         <f>K16*1.5</f>
         <v>18</v>
       </c>
-      <c r="K16" s="130">
+      <c r="K16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="L16" s="127"/>
-      <c r="M16" s="127"/>
-      <c r="N16" s="127" t="s">
-        <v>184</v>
-      </c>
-      <c r="O16" s="127"/>
+      <c r="N16" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="P16" s="45"/>
     </row>
     <row r="17" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="111"/>
-      <c r="B17" s="140"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="127"/>
-      <c r="E17" s="143" t="s">
+      <c r="B17" s="112"/>
+      <c r="E17" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="143"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="145" t="s">
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="146">
+      <c r="I17" s="65">
+        <f>I14/2</f>
         <v>10</v>
       </c>
-      <c r="J17" s="146">
+      <c r="J17" s="65">
         <f>K17*1.5</f>
         <v>3</v>
       </c>
-      <c r="K17" s="146">
+      <c r="K17" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L17" s="127"/>
-      <c r="M17" s="127"/>
-      <c r="N17" s="127" t="s">
-        <v>83</v>
-      </c>
-      <c r="O17" s="127"/>
+      <c r="N17" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="P17" s="45"/>
     </row>
     <row r="18" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44"/>
-      <c r="B18" s="127"/>
-      <c r="C18" s="127"/>
-      <c r="D18" s="127"/>
-      <c r="E18" s="138" t="s">
+      <c r="E18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="138"/>
-      <c r="G18" s="127"/>
-      <c r="H18" s="141" t="s">
+      <c r="F18" s="41"/>
+      <c r="H18" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="142">
+      <c r="I18" s="61">
+        <f>I14/2</f>
         <v>10</v>
       </c>
-      <c r="J18" s="130">
+      <c r="J18" s="1">
         <f>K18*1.5</f>
         <v>3</v>
       </c>
-      <c r="K18" s="130">
+      <c r="K18" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L18" s="127"/>
-      <c r="M18" s="127"/>
-      <c r="N18" s="127" t="s">
-        <v>210</v>
-      </c>
-      <c r="O18" s="127"/>
       <c r="P18" s="45"/>
     </row>
     <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2676,29 +2645,21 @@
         <v>87</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="127"/>
-      <c r="D19" s="127"/>
-      <c r="E19" s="143" t="s">
+      <c r="E19" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="143"/>
-      <c r="G19" s="144"/>
-      <c r="H19" s="145" t="s">
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="147" t="s">
-        <v>95</v>
-      </c>
-      <c r="J19" s="147" t="s">
-        <v>94</v>
-      </c>
-      <c r="K19" s="147"/>
-      <c r="L19" s="127"/>
-      <c r="M19" s="127"/>
-      <c r="N19" s="127" t="s">
-        <v>211</v>
-      </c>
-      <c r="O19" s="127"/>
+      <c r="I19" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="K19" s="66"/>
       <c r="P19" s="45"/>
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2708,21 +2669,8 @@
       <c r="B20" s="67">
         <v>0</v>
       </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
-      <c r="E20" s="127"/>
-      <c r="F20" s="127"/>
-      <c r="G20" s="127"/>
-      <c r="H20" s="127"/>
-      <c r="I20" s="127"/>
-      <c r="J20" s="127"/>
-      <c r="K20" s="127"/>
-      <c r="L20" s="127"/>
-      <c r="M20" s="127"/>
-      <c r="N20" s="148" t="s">
-        <v>149</v>
-      </c>
-      <c r="O20" s="148"/>
+      <c r="N20" s="103"/>
+      <c r="O20" s="103"/>
       <c r="P20" s="104"/>
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2732,25 +2680,14 @@
       <c r="B21" s="67">
         <v>500</v>
       </c>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="149" t="s">
+      <c r="E21" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="127"/>
-      <c r="G21" s="127"/>
-      <c r="H21" s="127"/>
-      <c r="I21" s="127"/>
-      <c r="J21" s="127"/>
-      <c r="K21" s="127"/>
-      <c r="L21" s="127"/>
-      <c r="M21" s="127"/>
-      <c r="N21" s="127"/>
-      <c r="O21" s="150" t="s">
+      <c r="O21" s="68" t="s">
         <v>48</v>
       </c>
       <c r="P21" s="69">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2760,21 +2697,11 @@
       <c r="B22" s="67">
         <v>0</v>
       </c>
-      <c r="C22" s="128"/>
-      <c r="D22" s="128"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="128"/>
-      <c r="G22" s="128"/>
-      <c r="H22" s="128"/>
-      <c r="I22" s="128"/>
-      <c r="J22" s="128"/>
-      <c r="K22" s="128"/>
-      <c r="L22" s="128"/>
-      <c r="M22" s="128"/>
-      <c r="N22" s="127"/>
-      <c r="O22" s="150" t="s">
+      <c r="N22" s="3"/>
+      <c r="O22" s="68" t="s">
         <v>41</v>
       </c>
       <c r="P22" s="69">
@@ -2788,101 +2715,53 @@
       <c r="B23" s="67">
         <v>0</v>
       </c>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128" t="s">
+      <c r="E23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="128"/>
-      <c r="K23" s="128"/>
-      <c r="L23" s="128"/>
-      <c r="M23" s="138"/>
-      <c r="N23" s="151"/>
-      <c r="O23" s="128"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="42"/>
       <c r="P23" s="55"/>
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="56"/>
-      <c r="B24" s="128"/>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128" t="s">
+      <c r="E24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F24" s="128"/>
-      <c r="G24" s="128"/>
-      <c r="H24" s="128"/>
-      <c r="I24" s="128"/>
-      <c r="J24" s="128"/>
-      <c r="K24" s="128"/>
-      <c r="L24" s="128"/>
-      <c r="M24" s="138"/>
-      <c r="N24" s="138"/>
-      <c r="O24" s="128"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
       <c r="P24" s="55"/>
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="56"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="128"/>
-      <c r="D25" s="128"/>
-      <c r="E25" s="128" t="s">
+      <c r="E25" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F25" s="128"/>
-      <c r="G25" s="128"/>
-      <c r="H25" s="128"/>
-      <c r="I25" s="128"/>
-      <c r="J25" s="128"/>
-      <c r="K25" s="128"/>
-      <c r="L25" s="128"/>
-      <c r="M25" s="128"/>
-      <c r="N25" s="128"/>
-      <c r="O25" s="128"/>
       <c r="P25" s="55"/>
     </row>
     <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="56"/>
-      <c r="B26" s="128"/>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128" t="s">
-        <v>155</v>
-      </c>
-      <c r="F26" s="128"/>
-      <c r="G26" s="128"/>
-      <c r="H26" s="128"/>
-      <c r="I26" s="128"/>
-      <c r="J26" s="128"/>
-      <c r="K26" s="128"/>
-      <c r="L26" s="128"/>
-      <c r="M26" s="128"/>
-      <c r="N26" s="128"/>
-      <c r="O26" s="128"/>
       <c r="P26" s="55"/>
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="115" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" s="152"/>
-      <c r="C27" s="152" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="128"/>
-      <c r="E27" s="142"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="142"/>
-      <c r="H27" s="128"/>
-      <c r="I27" s="142"/>
-      <c r="J27" s="128"/>
-      <c r="K27" s="128"/>
-      <c r="L27" s="128"/>
-      <c r="M27" s="128"/>
+      <c r="A27" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
       <c r="N27" s="4" t="s">
         <v>29</v>
       </c>
@@ -2890,117 +2769,50 @@
       <c r="P27" s="53"/>
     </row>
     <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="B28" s="153"/>
-      <c r="C28" s="154">
-        <v>2</v>
-      </c>
-      <c r="D28" s="128"/>
-      <c r="E28" s="128"/>
-      <c r="F28" s="128"/>
-      <c r="G28" s="128"/>
-      <c r="H28" s="128"/>
-      <c r="I28" s="128"/>
-      <c r="J28" s="128"/>
-      <c r="K28" s="128"/>
-      <c r="L28" s="128"/>
-      <c r="M28" s="128"/>
-      <c r="N28" s="128" t="s">
-        <v>77</v>
-      </c>
-      <c r="O28" s="128"/>
+      <c r="A28" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>217</v>
+      </c>
       <c r="P28" s="55"/>
     </row>
     <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="118" t="s">
-        <v>151</v>
-      </c>
-      <c r="B29" s="153"/>
-      <c r="C29" s="153">
-        <v>3</v>
-      </c>
-      <c r="D29" s="128"/>
-      <c r="E29" s="128"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="128"/>
-      <c r="I29" s="128"/>
-      <c r="J29" s="128"/>
-      <c r="K29" s="128"/>
-      <c r="L29" s="128"/>
-      <c r="M29" s="128"/>
-      <c r="N29" s="128" t="s">
+      <c r="A29" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O29" s="128"/>
       <c r="P29" s="55"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="118" t="s">
-        <v>181</v>
-      </c>
-      <c r="B30" s="153"/>
-      <c r="C30" s="153">
-        <v>3</v>
-      </c>
-      <c r="D30" s="128"/>
-      <c r="E30" s="128"/>
-      <c r="F30" s="128"/>
-      <c r="G30" s="128"/>
-      <c r="H30" s="128"/>
-      <c r="I30" s="128"/>
-      <c r="J30" s="128"/>
-      <c r="K30" s="128"/>
-      <c r="L30" s="128"/>
-      <c r="M30" s="128"/>
-      <c r="N30" s="128" t="s">
+      <c r="A30" s="97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="128"/>
       <c r="P30" s="55"/>
     </row>
     <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="118" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="153"/>
-      <c r="C31" s="153">
-        <v>3</v>
-      </c>
-      <c r="D31" s="128"/>
-      <c r="E31" s="128"/>
-      <c r="F31" s="128"/>
-      <c r="G31" s="128"/>
-      <c r="H31" s="128"/>
-      <c r="I31" s="128"/>
-      <c r="J31" s="128"/>
-      <c r="K31" s="128"/>
-      <c r="L31" s="128"/>
-      <c r="M31" s="128"/>
-      <c r="N31" s="128" t="s">
-        <v>205</v>
-      </c>
-      <c r="O31" s="128"/>
+      <c r="A31" s="119"/>
+      <c r="N31" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="P31" s="55"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="56"/>
-      <c r="B32" s="128"/>
-      <c r="C32" s="128"/>
-      <c r="D32" s="128"/>
-      <c r="E32" s="128"/>
-      <c r="F32" s="128"/>
-      <c r="G32" s="128"/>
-      <c r="H32" s="128"/>
-      <c r="I32" s="128"/>
-      <c r="J32" s="128"/>
-      <c r="K32" s="128"/>
-      <c r="L32" s="128"/>
-      <c r="M32" s="128"/>
-      <c r="N32" s="128"/>
-      <c r="O32" s="128"/>
       <c r="P32" s="55"/>
     </row>
     <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
@@ -3059,120 +2871,115 @@
     </row>
     <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="B34" s="130" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="155">
+      <c r="C34" s="72">
+        <v>6</v>
+      </c>
+      <c r="D34" s="73">
+        <f>C34+1</f>
         <v>7</v>
       </c>
-      <c r="D34" s="156">
-        <f>C34+1</f>
+      <c r="E34" s="72">
+        <f t="shared" ref="E34:L34" si="2">D34+1</f>
         <v>8</v>
       </c>
-      <c r="E34" s="155">
-        <f t="shared" ref="E34:L34" si="2">D34+1</f>
+      <c r="F34" s="73">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="F34" s="156">
+      <c r="G34" s="72">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="G34" s="155">
+      <c r="H34" s="73">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="H34" s="156">
+      <c r="I34" s="72">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="I34" s="155">
+      <c r="J34" s="73">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="J34" s="156">
+      <c r="K34" s="72">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="K34" s="155">
+      <c r="L34" s="73">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="L34" s="156">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
       <c r="M34" s="106" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="N34" s="106"/>
-      <c r="O34" s="128" t="s">
-        <v>209</v>
-      </c>
       <c r="P34" s="55"/>
     </row>
     <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="130" t="s">
+      <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="155">
+      <c r="C35" s="72">
+        <v>6</v>
+      </c>
+      <c r="D35" s="73">
+        <f t="shared" ref="D35:L36" si="3">C35+1</f>
         <v>7</v>
       </c>
-      <c r="D35" s="156">
-        <f t="shared" ref="D35:L36" si="3">C35+1</f>
+      <c r="E35" s="72">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="E35" s="155">
+      <c r="F35" s="73">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="F35" s="156">
+      <c r="G35" s="72">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="G35" s="155">
+      <c r="H35" s="73">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="H35" s="156">
+      <c r="I35" s="72">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="I35" s="155">
+      <c r="J35" s="73">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="J35" s="156">
+      <c r="K35" s="72">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="K35" s="155">
+      <c r="L35" s="73">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="L35" s="156">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="M35" s="157" t="s">
-        <v>208</v>
-      </c>
-      <c r="N35" s="157"/>
-      <c r="O35" s="127" t="s">
-        <v>147</v>
-      </c>
+      <c r="M35" s="107" t="s">
+        <v>137</v>
+      </c>
+      <c r="N35" s="107"/>
+      <c r="O35" s="3"/>
       <c r="P35" s="55"/>
     </row>
     <row r="36" spans="1:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="74" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="C36" s="76">
         <v>8</v>
@@ -3217,9 +3024,7 @@
         <v>28</v>
       </c>
       <c r="N36" s="108"/>
-      <c r="O36" s="78" t="s">
-        <v>148</v>
-      </c>
+      <c r="O36" s="78"/>
       <c r="P36" s="79"/>
       <c r="AA36"/>
     </row>
@@ -3249,11 +3054,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E67570B-E252-4754-963B-16F0C4F39BE1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06982626-440A-421A-816A-4B07BD0E71A6}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3271,14 +3076,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="82" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="C1" s="82"/>
       <c r="D1" s="83"/>
       <c r="E1" s="99"/>
       <c r="F1" s="84"/>
       <c r="G1" s="101" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="H1" s="82"/>
       <c r="I1" s="84"/>
@@ -3299,27 +3104,27 @@
         <v>120</v>
       </c>
       <c r="B2" s="90" t="s">
-        <v>100</v>
+        <v>199</v>
       </c>
       <c r="C2" s="90"/>
-      <c r="D2" s="91"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="92" t="s">
         <v>33</v>
       </c>
       <c r="F2" s="93"/>
       <c r="G2" s="93" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="H2" s="93"/>
       <c r="I2" s="100" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" s="91"/>
-      <c r="K2" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="124"/>
+      <c r="K2" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
       <c r="N2" s="90" t="s">
         <v>72</v>
       </c>
@@ -3328,54 +3133,56 @@
     </row>
     <row r="3" spans="1:16" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="127"/>
+      <c r="O3" s="127"/>
       <c r="P3" s="45"/>
     </row>
     <row r="4" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="47">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="48" t="s">
+      <c r="B4" s="129">
+        <v>2</v>
+      </c>
+      <c r="C4" s="130"/>
+      <c r="D4" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="49">
-        <v>20</v>
-      </c>
-      <c r="G4" s="102" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="50" t="s">
+      <c r="E4" s="130"/>
+      <c r="F4" s="132">
+        <v>22</v>
+      </c>
+      <c r="G4" s="133" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="134" t="s">
         <v>119</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="51">
-        <v>2</v>
-      </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="48" t="s">
+      <c r="L4" s="130"/>
+      <c r="M4" s="135">
+        <v>0</v>
+      </c>
+      <c r="N4" s="130"/>
+      <c r="O4" s="131" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="98">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3383,9 +3190,18 @@
         <v>29</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="J5" s="2" t="s">
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128" t="s">
         <v>118</v>
       </c>
+      <c r="K5" s="128"/>
+      <c r="L5" s="128"/>
       <c r="M5" s="7" t="s">
         <v>10</v>
       </c>
@@ -3395,173 +3211,196 @@
     </row>
     <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="80">
-        <v>9</v>
-      </c>
-      <c r="B6" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="109" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="49">
-        <v>0</v>
-      </c>
-      <c r="K6" s="49"/>
-      <c r="M6" s="110" t="s">
+      <c r="C6" s="136" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="132">
+        <v>1</v>
+      </c>
+      <c r="K6" s="132"/>
+      <c r="L6" s="128"/>
+      <c r="M6" s="137" t="s">
         <v>73</v>
       </c>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
+      <c r="N6" s="137"/>
+      <c r="O6" s="137"/>
       <c r="P6" s="54">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="80">
-        <v>16</v>
-      </c>
-      <c r="B7" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="109" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="49">
-        <v>2</v>
-      </c>
-      <c r="K7" s="49"/>
-      <c r="M7" s="110" t="s">
+      <c r="C7" s="136" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="136"/>
+      <c r="I7" s="136"/>
+      <c r="J7" s="132">
+        <v>0</v>
+      </c>
+      <c r="K7" s="132"/>
+      <c r="L7" s="128"/>
+      <c r="M7" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="110"/>
-      <c r="O7" s="110"/>
+      <c r="N7" s="137"/>
+      <c r="O7" s="137"/>
       <c r="P7" s="54">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="80">
-        <v>13</v>
-      </c>
-      <c r="B8" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="136" t="s">
         <v>161</v>
       </c>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="49">
-        <v>1</v>
-      </c>
-      <c r="K8" s="49"/>
-      <c r="M8" s="110" t="s">
+      <c r="D8" s="136"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="136"/>
+      <c r="J8" s="132">
+        <v>2</v>
+      </c>
+      <c r="K8" s="132"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
+      <c r="N8" s="137"/>
+      <c r="O8" s="137"/>
       <c r="P8" s="54">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="80">
-        <v>14</v>
-      </c>
-      <c r="B9" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="109" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="49">
-        <v>1</v>
-      </c>
-      <c r="K9" s="49"/>
-      <c r="M9" s="110" t="s">
+      <c r="C9" s="136" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="136"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="132">
+        <v>0</v>
+      </c>
+      <c r="K9" s="132"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="110"/>
-      <c r="O9" s="110"/>
+      <c r="N9" s="137"/>
+      <c r="O9" s="137"/>
       <c r="P9" s="54">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="80">
+        <v>13</v>
+      </c>
+      <c r="B10" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="109" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="49">
-        <v>-1</v>
-      </c>
-      <c r="K10" s="49"/>
-      <c r="M10" s="110" t="s">
+      <c r="C10" s="136" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="136"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="136"/>
+      <c r="J10" s="132">
+        <v>1</v>
+      </c>
+      <c r="K10" s="132"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="110"/>
-      <c r="O10" s="110"/>
+      <c r="N10" s="137"/>
+      <c r="O10" s="137"/>
       <c r="P10" s="54">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="80">
-        <v>10</v>
-      </c>
-      <c r="B11" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="136" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="49">
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="132">
         <v>0</v>
       </c>
-      <c r="K11" s="49"/>
+      <c r="K11" s="132"/>
+      <c r="L11" s="128"/>
+      <c r="M11" s="128"/>
+      <c r="N11" s="128"/>
+      <c r="O11" s="128"/>
       <c r="P11" s="55"/>
     </row>
     <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="56"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="128"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
+      <c r="J12" s="128"/>
+      <c r="K12" s="128"/>
+      <c r="L12" s="128"/>
+      <c r="M12" s="128"/>
+      <c r="N12" s="128"/>
+      <c r="O12" s="128"/>
       <c r="P12" s="55"/>
     </row>
     <row r="13" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3569,22 +3408,25 @@
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="41"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="127"/>
       <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="58" t="s">
+      <c r="H13" s="138"/>
+      <c r="I13" s="139" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="139" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="139" t="s">
         <v>93</v>
       </c>
+      <c r="L13" s="127"/>
+      <c r="M13" s="127"/>
       <c r="N13" s="4" t="s">
         <v>79</v>
       </c>
@@ -3593,139 +3435,164 @@
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="B14" s="112"/>
-      <c r="E14" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" s="140"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="41"/>
-      <c r="H14" s="60" t="s">
+      <c r="F14" s="138"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="141" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="61">
-        <v>40</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="I14" s="142">
+        <v>20</v>
+      </c>
+      <c r="J14" s="130">
         <f>K14*1.5</f>
-        <v>12</v>
-      </c>
-      <c r="K14" s="1">
+        <v>6</v>
+      </c>
+      <c r="K14" s="130">
         <f>I14/5</f>
-        <v>8</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>183</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="L14" s="127"/>
+      <c r="M14" s="127"/>
+      <c r="N14" s="127" t="s">
+        <v>80</v>
+      </c>
+      <c r="O14" s="127"/>
       <c r="P14" s="45"/>
     </row>
     <row r="15" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="111"/>
-      <c r="B15" s="112"/>
-      <c r="E15" s="62" t="s">
+      <c r="B15" s="140"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="64" t="s">
+      <c r="F15" s="143"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="145" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="65">
-        <f>I14*3</f>
-        <v>120</v>
-      </c>
-      <c r="J15" s="65">
+      <c r="I15" s="146">
+        <v>60</v>
+      </c>
+      <c r="J15" s="146">
         <f>K15*1.5</f>
-        <v>36</v>
-      </c>
-      <c r="K15" s="65">
+        <v>18</v>
+      </c>
+      <c r="K15" s="146">
         <f t="shared" ref="K15:K18" si="0">I15/5</f>
-        <v>24</v>
-      </c>
-      <c r="N15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="127"/>
+      <c r="M15" s="127"/>
+      <c r="N15" s="127" t="s">
         <v>167</v>
       </c>
+      <c r="O15" s="127"/>
       <c r="P15" s="45"/>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="111"/>
-      <c r="B16" s="112"/>
-      <c r="E16" s="41" t="s">
+      <c r="B16" s="140"/>
+      <c r="C16" s="127"/>
+      <c r="D16" s="127"/>
+      <c r="E16" s="138" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="H16" s="60" t="s">
+      <c r="F16" s="138"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="141" t="s">
         <v>96</v>
       </c>
-      <c r="I16" s="61">
-        <f>I14*3</f>
-        <v>120</v>
-      </c>
-      <c r="J16" s="1">
+      <c r="I16" s="142">
+        <v>60</v>
+      </c>
+      <c r="J16" s="130">
         <f>K16*1.5</f>
-        <v>36</v>
-      </c>
-      <c r="K16" s="1">
+        <v>18</v>
+      </c>
+      <c r="K16" s="130">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="N16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="127" t="s">
         <v>184</v>
       </c>
+      <c r="O16" s="127"/>
       <c r="P16" s="45"/>
     </row>
     <row r="17" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="111"/>
-      <c r="B17" s="112"/>
-      <c r="E17" s="62" t="s">
+      <c r="B17" s="140"/>
+      <c r="C17" s="127"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="143" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="62"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="64" t="s">
+      <c r="F17" s="143"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="145" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="65">
-        <f>I14/2</f>
-        <v>20</v>
-      </c>
-      <c r="J17" s="65">
+      <c r="I17" s="146">
+        <v>10</v>
+      </c>
+      <c r="J17" s="146">
         <f>K17*1.5</f>
-        <v>6</v>
-      </c>
-      <c r="K17" s="65">
+        <v>3</v>
+      </c>
+      <c r="K17" s="146">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="N17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="127"/>
+      <c r="M17" s="127"/>
+      <c r="N17" s="127" t="s">
         <v>83</v>
       </c>
+      <c r="O17" s="127"/>
       <c r="P17" s="45"/>
     </row>
     <row r="18" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44"/>
-      <c r="E18" s="41" t="s">
+      <c r="B18" s="127"/>
+      <c r="C18" s="127"/>
+      <c r="D18" s="127"/>
+      <c r="E18" s="138" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="41"/>
-      <c r="H18" s="60" t="s">
+      <c r="F18" s="138"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="141" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="61">
-        <f>I14/2</f>
-        <v>20</v>
-      </c>
-      <c r="J18" s="1">
+      <c r="I18" s="142">
+        <v>10</v>
+      </c>
+      <c r="J18" s="130">
         <f>K18*1.5</f>
-        <v>6</v>
-      </c>
-      <c r="K18" s="1">
+        <v>3</v>
+      </c>
+      <c r="K18" s="130">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>185</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L18" s="127"/>
+      <c r="M18" s="127"/>
+      <c r="N18" s="127" t="s">
+        <v>210</v>
+      </c>
+      <c r="O18" s="127"/>
       <c r="P18" s="45"/>
     </row>
     <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3733,24 +3600,29 @@
         <v>87</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="E19" s="62" t="s">
+      <c r="C19" s="127"/>
+      <c r="D19" s="127"/>
+      <c r="E19" s="143" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="64" t="s">
+      <c r="F19" s="143"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="145" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="66" t="s">
-        <v>165</v>
-      </c>
-      <c r="J19" s="66" t="s">
-        <v>164</v>
-      </c>
-      <c r="K19" s="66"/>
-      <c r="N19" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="I19" s="147" t="s">
+        <v>95</v>
+      </c>
+      <c r="J19" s="147" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" s="147"/>
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="127" t="s">
+        <v>211</v>
+      </c>
+      <c r="O19" s="127"/>
       <c r="P19" s="45"/>
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3760,10 +3632,21 @@
       <c r="B20" s="67">
         <v>0</v>
       </c>
-      <c r="N20" s="103" t="s">
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="127"/>
+      <c r="K20" s="127"/>
+      <c r="L20" s="127"/>
+      <c r="M20" s="127"/>
+      <c r="N20" s="148" t="s">
         <v>149</v>
       </c>
-      <c r="O20" s="103"/>
+      <c r="O20" s="148"/>
       <c r="P20" s="104"/>
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3773,14 +3656,25 @@
       <c r="B21" s="67">
         <v>500</v>
       </c>
-      <c r="E21" t="s">
+      <c r="C21" s="127"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="149" t="s">
         <v>40</v>
       </c>
-      <c r="O21" s="68" t="s">
+      <c r="F21" s="127"/>
+      <c r="G21" s="127"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="127"/>
+      <c r="J21" s="127"/>
+      <c r="K21" s="127"/>
+      <c r="L21" s="127"/>
+      <c r="M21" s="127"/>
+      <c r="N21" s="127"/>
+      <c r="O21" s="150" t="s">
         <v>48</v>
       </c>
       <c r="P21" s="69">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3790,11 +3684,21 @@
       <c r="B22" s="67">
         <v>0</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="128" t="s">
         <v>122</v>
       </c>
-      <c r="N22" s="3"/>
-      <c r="O22" s="68" t="s">
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="128"/>
+      <c r="J22" s="128"/>
+      <c r="K22" s="128"/>
+      <c r="L22" s="128"/>
+      <c r="M22" s="128"/>
+      <c r="N22" s="127"/>
+      <c r="O22" s="150" t="s">
         <v>41</v>
       </c>
       <c r="P22" s="69">
@@ -3808,57 +3712,101 @@
       <c r="B23" s="67">
         <v>0</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128" t="s">
         <v>124</v>
       </c>
-      <c r="M23" s="41"/>
-      <c r="N23" s="42"/>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
+      <c r="J23" s="128"/>
+      <c r="K23" s="128"/>
+      <c r="L23" s="128"/>
+      <c r="M23" s="138"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="128"/>
       <c r="P23" s="55"/>
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="56"/>
-      <c r="E24" s="2" t="s">
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128" t="s">
         <v>125</v>
       </c>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="128"/>
+      <c r="L24" s="128"/>
+      <c r="M24" s="138"/>
+      <c r="N24" s="138"/>
+      <c r="O24" s="128"/>
       <c r="P24" s="55"/>
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="121" t="s">
-        <v>189</v>
-      </c>
-      <c r="C25" s="123">
-        <v>0.45</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="A25" s="56"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128" t="s">
         <v>123</v>
       </c>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="128"/>
+      <c r="L25" s="128"/>
+      <c r="M25" s="128"/>
+      <c r="N25" s="128"/>
+      <c r="O25" s="128"/>
       <c r="P25" s="55"/>
     </row>
     <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="122" t="s">
-        <v>194</v>
-      </c>
-      <c r="C26" s="123">
-        <v>0.4</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="A26" s="56"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128" t="s">
         <v>155</v>
       </c>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="128"/>
+      <c r="L26" s="128"/>
+      <c r="M26" s="128"/>
+      <c r="N26" s="128"/>
+      <c r="O26" s="128"/>
       <c r="P26" s="55"/>
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="118" t="s">
-        <v>190</v>
-      </c>
-      <c r="B27" s="114"/>
-      <c r="C27" s="123">
-        <v>0.45</v>
-      </c>
-      <c r="E27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="I27" s="61"/>
+      <c r="A27" s="115" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="152"/>
+      <c r="C27" s="152" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="128"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="128"/>
       <c r="N27" s="4" t="s">
         <v>29</v>
       </c>
@@ -3866,59 +3814,117 @@
       <c r="P27" s="53"/>
     </row>
     <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="116" t="s">
-        <v>191</v>
-      </c>
-      <c r="B28" s="117"/>
-      <c r="C28" s="123">
-        <v>0.45</v>
-      </c>
-      <c r="E28" s="120" t="s">
-        <v>196</v>
-      </c>
-      <c r="N28" s="2" t="s">
+      <c r="A28" s="118" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="153"/>
+      <c r="C28" s="154">
+        <v>2</v>
+      </c>
+      <c r="D28" s="128"/>
+      <c r="E28" s="128"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="128"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="128"/>
+      <c r="J28" s="128"/>
+      <c r="K28" s="128"/>
+      <c r="L28" s="128"/>
+      <c r="M28" s="128"/>
+      <c r="N28" s="128" t="s">
         <v>77</v>
       </c>
+      <c r="O28" s="128"/>
       <c r="P28" s="55"/>
     </row>
     <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="116" t="s">
-        <v>192</v>
-      </c>
-      <c r="B29" s="117"/>
-      <c r="C29" s="123">
-        <v>0.92</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>187</v>
-      </c>
+      <c r="A29" s="118" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="153"/>
+      <c r="C29" s="153">
+        <v>3</v>
+      </c>
+      <c r="D29" s="128"/>
+      <c r="E29" s="128"/>
+      <c r="F29" s="128"/>
+      <c r="G29" s="128"/>
+      <c r="H29" s="128"/>
+      <c r="I29" s="128"/>
+      <c r="J29" s="128"/>
+      <c r="K29" s="128"/>
+      <c r="L29" s="128"/>
+      <c r="M29" s="128"/>
+      <c r="N29" s="128" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29" s="128"/>
       <c r="P29" s="55"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="118" t="s">
-        <v>193</v>
-      </c>
-      <c r="B30" s="117"/>
-      <c r="C30" s="123">
-        <v>0.36</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>188</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="B30" s="153"/>
+      <c r="C30" s="153">
+        <v>3</v>
+      </c>
+      <c r="D30" s="128"/>
+      <c r="E30" s="128"/>
+      <c r="F30" s="128"/>
+      <c r="G30" s="128"/>
+      <c r="H30" s="128"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="128"/>
+      <c r="K30" s="128"/>
+      <c r="L30" s="128"/>
+      <c r="M30" s="128"/>
+      <c r="N30" s="128" t="s">
+        <v>78</v>
+      </c>
+      <c r="O30" s="128"/>
       <c r="P30" s="55"/>
     </row>
     <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="118" t="s">
-        <v>195</v>
-      </c>
-      <c r="B31" s="117"/>
-      <c r="C31" s="123">
-        <v>0.8</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B31" s="153"/>
+      <c r="C31" s="153">
+        <v>3</v>
+      </c>
+      <c r="D31" s="128"/>
+      <c r="E31" s="128"/>
+      <c r="F31" s="128"/>
+      <c r="G31" s="128"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="128"/>
+      <c r="J31" s="128"/>
+      <c r="K31" s="128"/>
+      <c r="L31" s="128"/>
+      <c r="M31" s="128"/>
+      <c r="N31" s="128" t="s">
+        <v>205</v>
+      </c>
+      <c r="O31" s="128"/>
       <c r="P31" s="55"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="56"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="128"/>
+      <c r="H32" s="128"/>
+      <c r="I32" s="128"/>
+      <c r="J32" s="128"/>
+      <c r="K32" s="128"/>
+      <c r="L32" s="128"/>
+      <c r="M32" s="128"/>
+      <c r="N32" s="128"/>
+      <c r="O32" s="128"/>
       <c r="P32" s="55"/>
     </row>
     <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
@@ -3977,107 +3983,110 @@
     </row>
     <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="71" t="s">
-        <v>180</v>
-      </c>
-      <c r="B34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="72">
+      <c r="C34" s="155">
+        <v>7</v>
+      </c>
+      <c r="D34" s="156">
+        <f>C34+1</f>
         <v>8</v>
       </c>
-      <c r="D34" s="73">
-        <f>C34+1</f>
+      <c r="E34" s="155">
+        <f t="shared" ref="E34:L34" si="2">D34+1</f>
         <v>9</v>
       </c>
-      <c r="E34" s="72">
-        <f t="shared" ref="E34:L34" si="2">D34+1</f>
+      <c r="F34" s="156">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="F34" s="73">
+      <c r="G34" s="155">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="G34" s="72">
+      <c r="H34" s="156">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="H34" s="73">
+      <c r="I34" s="155">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="I34" s="72">
+      <c r="J34" s="156">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="J34" s="73">
+      <c r="K34" s="155">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="K34" s="72">
+      <c r="L34" s="156">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="L34" s="73">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
       <c r="M34" s="106" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="N34" s="106"/>
+      <c r="O34" s="128" t="s">
+        <v>209</v>
+      </c>
       <c r="P34" s="55"/>
     </row>
     <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="72">
+      <c r="C35" s="155">
+        <v>7</v>
+      </c>
+      <c r="D35" s="156">
+        <f t="shared" ref="D35:L36" si="3">C35+1</f>
         <v>8</v>
       </c>
-      <c r="D35" s="73">
-        <f t="shared" ref="D35:L36" si="3">C35+1</f>
+      <c r="E35" s="155">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="E35" s="72">
+      <c r="F35" s="156">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="F35" s="73">
+      <c r="G35" s="155">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="G35" s="72">
+      <c r="H35" s="156">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="H35" s="73">
+      <c r="I35" s="155">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="I35" s="72">
+      <c r="J35" s="156">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="J35" s="73">
+      <c r="K35" s="155">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="K35" s="72">
+      <c r="L35" s="156">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="L35" s="73">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="M35" s="107" t="s">
-        <v>110</v>
-      </c>
-      <c r="N35" s="107"/>
-      <c r="O35" s="3" t="s">
+      <c r="M35" s="157" t="s">
+        <v>208</v>
+      </c>
+      <c r="N35" s="157"/>
+      <c r="O35" s="127" t="s">
         <v>147</v>
       </c>
       <c r="P35" s="55"/>
@@ -4087,46 +4096,46 @@
         <v>181</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="C36" s="76">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D36" s="77">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E36" s="76">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F36" s="77">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G36" s="76">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H36" s="77">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I36" s="76">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J36" s="77">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K36" s="76">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L36" s="77">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M36" s="108" t="s">
         <v>28</v>
@@ -4164,11 +4173,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23066C9D-052A-4A0F-9F62-A1EE62475AEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E67570B-E252-4754-963B-16F0C4F39BE1}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4186,14 +4195,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="82" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="C1" s="82"/>
       <c r="D1" s="83"/>
       <c r="E1" s="99"/>
       <c r="F1" s="84"/>
       <c r="G1" s="101" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="H1" s="82"/>
       <c r="I1" s="84"/>
@@ -4223,11 +4232,11 @@
       </c>
       <c r="F2" s="93"/>
       <c r="G2" s="93" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="H2" s="93"/>
       <c r="I2" s="100" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="J2" s="91"/>
       <c r="K2" s="94" t="s">
@@ -4262,7 +4271,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="47">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="48" t="s">
@@ -4270,10 +4279,10 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="49">
-        <v>18</v>
-      </c>
-      <c r="G4" s="49">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="G4" s="102" t="s">
+        <v>88</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -4283,14 +4292,14 @@
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="48" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="98">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4310,13 +4319,13 @@
     </row>
     <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="80">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="50" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="109" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="D6" s="109"/>
       <c r="E6" s="109"/>
@@ -4325,7 +4334,7 @@
       <c r="H6" s="109"/>
       <c r="I6" s="109"/>
       <c r="J6" s="49">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="49"/>
       <c r="M6" s="110" t="s">
@@ -4334,18 +4343,18 @@
       <c r="N6" s="110"/>
       <c r="O6" s="110"/>
       <c r="P6" s="54">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="80">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="109" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="D7" s="109"/>
       <c r="E7" s="109"/>
@@ -4354,7 +4363,7 @@
       <c r="H7" s="109"/>
       <c r="I7" s="109"/>
       <c r="J7" s="49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" s="49"/>
       <c r="M7" s="110" t="s">
@@ -4363,7 +4372,7 @@
       <c r="N7" s="110"/>
       <c r="O7" s="110"/>
       <c r="P7" s="54">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4392,12 +4401,12 @@
       <c r="N8" s="110"/>
       <c r="O8" s="110"/>
       <c r="P8" s="54">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="80">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="50" t="s">
         <v>5</v>
@@ -4412,7 +4421,7 @@
       <c r="H9" s="109"/>
       <c r="I9" s="109"/>
       <c r="J9" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9" s="49"/>
       <c r="M9" s="110" t="s">
@@ -4426,13 +4435,13 @@
     </row>
     <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="80">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="109" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="D10" s="109"/>
       <c r="E10" s="109"/>
@@ -4441,7 +4450,7 @@
       <c r="H10" s="109"/>
       <c r="I10" s="109"/>
       <c r="J10" s="49">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K10" s="49"/>
       <c r="M10" s="110" t="s">
@@ -4450,18 +4459,18 @@
       <c r="N10" s="110"/>
       <c r="O10" s="110"/>
       <c r="P10" s="54">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="80">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="50" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="109" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="D11" s="109"/>
       <c r="E11" s="109"/>
@@ -4470,7 +4479,7 @@
       <c r="H11" s="109"/>
       <c r="I11" s="109"/>
       <c r="J11" s="49">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="49"/>
       <c r="P11" s="55"/>
@@ -4508,7 +4517,7 @@
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="111" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="B14" s="112"/>
       <c r="E14" s="41" t="s">
@@ -4530,7 +4539,7 @@
         <v>8</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="P14" s="45"/>
     </row>
@@ -4585,7 +4594,7 @@
         <v>24</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>83</v>
+        <v>184</v>
       </c>
       <c r="P16" s="45"/>
     </row>
@@ -4613,7 +4622,7 @@
         <v>4</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>168</v>
+        <v>83</v>
       </c>
       <c r="P17" s="45"/>
     </row>
@@ -4638,6 +4647,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="N18" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="P18" s="45"/>
     </row>
     <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -4660,6 +4672,9 @@
         <v>164</v>
       </c>
       <c r="K19" s="66"/>
+      <c r="N19" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="P19" s="45"/>
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -4669,7 +4684,9 @@
       <c r="B20" s="67">
         <v>0</v>
       </c>
-      <c r="N20" s="103"/>
+      <c r="N20" s="103" t="s">
+        <v>149</v>
+      </c>
       <c r="O20" s="103"/>
       <c r="P20" s="104"/>
     </row>
@@ -4687,7 +4704,7 @@
         <v>48</v>
       </c>
       <c r="P21" s="69">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -4732,36 +4749,40 @@
       <c r="P24" s="55"/>
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
+      <c r="A25" s="121" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="123">
+        <v>0.45</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>123</v>
       </c>
       <c r="P25" s="55"/>
     </row>
     <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="56"/>
+      <c r="A26" s="122" t="s">
+        <v>194</v>
+      </c>
+      <c r="C26" s="123">
+        <v>0.4</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="P26" s="55"/>
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="A27" s="118" t="s">
+        <v>190</v>
+      </c>
+      <c r="B27" s="114"/>
+      <c r="C27" s="123">
+        <v>0.45</v>
+      </c>
+      <c r="E27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="I27" s="61"/>
       <c r="N27" s="4" t="s">
         <v>29</v>
       </c>
@@ -4769,11 +4790,15 @@
       <c r="P27" s="53"/>
     </row>
     <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="97" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>173</v>
+      <c r="A28" s="116" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="117"/>
+      <c r="C28" s="123">
+        <v>0.45</v>
+      </c>
+      <c r="E28" s="120" t="s">
+        <v>196</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>77</v>
@@ -4781,31 +4806,39 @@
       <c r="P28" s="55"/>
     </row>
     <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>174</v>
+      <c r="A29" s="116" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" s="117"/>
+      <c r="C29" s="123">
+        <v>0.92</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="P29" s="55"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="97" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>172</v>
+      <c r="A30" s="118" t="s">
+        <v>193</v>
+      </c>
+      <c r="B30" s="117"/>
+      <c r="C30" s="123">
+        <v>0.36</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="P30" s="55"/>
     </row>
     <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="119"/>
+      <c r="A31" s="118" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" s="117"/>
+      <c r="C31" s="123">
+        <v>0.8</v>
+      </c>
       <c r="P31" s="55"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -4868,52 +4901,52 @@
     </row>
     <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="71" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C34" s="72">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D34" s="73">
         <f>C34+1</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E34" s="72">
         <f t="shared" ref="E34:L34" si="2">D34+1</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F34" s="73">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G34" s="72">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H34" s="73">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I34" s="72">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J34" s="73">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K34" s="72">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L34" s="73">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M34" s="106" t="s">
-        <v>170</v>
+        <v>107</v>
       </c>
       <c r="N34" s="106"/>
       <c r="P34" s="55"/>
@@ -4926,102 +4959,106 @@
         <v>23</v>
       </c>
       <c r="C35" s="72">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D35" s="73">
         <f t="shared" ref="D35:L36" si="3">C35+1</f>
+        <v>9</v>
+      </c>
+      <c r="E35" s="72">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F35" s="73">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G35" s="72">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="E35" s="72">
+      <c r="H35" s="73">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="F35" s="73">
+      <c r="I35" s="72">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="G35" s="72">
+      <c r="J35" s="73">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="H35" s="73">
+      <c r="K35" s="72">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="I35" s="72">
+      <c r="L35" s="73">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="J35" s="73">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="K35" s="72">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="L35" s="73">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
       <c r="M35" s="107" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="N35" s="107"/>
-      <c r="O35" s="3"/>
+      <c r="O35" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="P35" s="55"/>
     </row>
     <row r="36" spans="1:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="74" t="s">
-        <v>24</v>
+        <v>181</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C36" s="76">
+        <v>6</v>
+      </c>
+      <c r="D36" s="77">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E36" s="76">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="F36" s="77">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G36" s="76">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="D36" s="77">
+      <c r="H36" s="77">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="E36" s="76">
+      <c r="I36" s="76">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="F36" s="77">
+      <c r="J36" s="77">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="G36" s="76">
+      <c r="K36" s="76">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="H36" s="77">
+      <c r="L36" s="77">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="I36" s="76">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="J36" s="77">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="K36" s="76">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="L36" s="77">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
       <c r="M36" s="108" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="N36" s="108"/>
-      <c r="O36" s="78"/>
+      <c r="O36" s="78" t="s">
+        <v>148</v>
+      </c>
       <c r="P36" s="79"/>
       <c r="AA36"/>
     </row>
@@ -5051,11 +5088,898 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23066C9D-052A-4A0F-9F62-A1EE62475AEE}">
+  <dimension ref="A1:AA36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="2" customWidth="1"/>
+    <col min="3" max="12" width="4.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="4.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="82"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="82"/>
+      <c r="P1" s="88"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="93"/>
+      <c r="I2" s="100" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="91"/>
+      <c r="K2" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="90"/>
+      <c r="P2" s="96"/>
+    </row>
+    <row r="3" spans="1:16" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="44"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="45"/>
+    </row>
+    <row r="4" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="47">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="49">
+        <v>18</v>
+      </c>
+      <c r="G4" s="49">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="51">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="98">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="J5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="53"/>
+    </row>
+    <row r="6" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="80">
+        <v>8</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="109" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="49">
+        <v>-1</v>
+      </c>
+      <c r="K6" s="49"/>
+      <c r="M6" s="110" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="80">
+        <v>10</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="49">
+        <v>0</v>
+      </c>
+      <c r="K7" s="49"/>
+      <c r="M7" s="110" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="110"/>
+      <c r="O7" s="110"/>
+      <c r="P7" s="54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="80">
+        <v>13</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="109" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="49">
+        <v>1</v>
+      </c>
+      <c r="K8" s="49"/>
+      <c r="M8" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="80">
+        <v>16</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="109" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="49">
+        <v>2</v>
+      </c>
+      <c r="K9" s="49"/>
+      <c r="M9" s="110" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="80">
+        <v>9</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="49">
+        <v>0</v>
+      </c>
+      <c r="K10" s="49"/>
+      <c r="M10" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="110"/>
+      <c r="O10" s="110"/>
+      <c r="P10" s="54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="80">
+        <v>8</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="109" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="49">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="49"/>
+      <c r="P11" s="55"/>
+    </row>
+    <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="56"/>
+      <c r="P12" s="55"/>
+    </row>
+    <row r="13" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="41"/>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" s="5"/>
+      <c r="P13" s="59"/>
+    </row>
+    <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="111" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="112"/>
+      <c r="E14" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="41"/>
+      <c r="H14" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="61">
+        <v>40</v>
+      </c>
+      <c r="J14" s="1">
+        <f>K14*1.5</f>
+        <v>12</v>
+      </c>
+      <c r="K14" s="1">
+        <f>I14/5</f>
+        <v>8</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="P14" s="45"/>
+    </row>
+    <row r="15" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="111"/>
+      <c r="B15" s="112"/>
+      <c r="E15" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="65">
+        <f>I14*3</f>
+        <v>120</v>
+      </c>
+      <c r="J15" s="65">
+        <f>K15*1.5</f>
+        <v>36</v>
+      </c>
+      <c r="K15" s="65">
+        <f t="shared" ref="K15:K18" si="0">I15/5</f>
+        <v>24</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P15" s="45"/>
+    </row>
+    <row r="16" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112"/>
+      <c r="E16" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="H16" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" s="61">
+        <f>I14*3</f>
+        <v>120</v>
+      </c>
+      <c r="J16" s="1">
+        <f>K16*1.5</f>
+        <v>36</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P16" s="45"/>
+    </row>
+    <row r="17" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="111"/>
+      <c r="B17" s="112"/>
+      <c r="E17" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="65">
+        <f>I14/2</f>
+        <v>20</v>
+      </c>
+      <c r="J17" s="65">
+        <f>K17*1.5</f>
+        <v>6</v>
+      </c>
+      <c r="K17" s="65">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="P17" s="45"/>
+    </row>
+    <row r="18" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44"/>
+      <c r="E18" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="41"/>
+      <c r="H18" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="61">
+        <f>I14/2</f>
+        <v>20</v>
+      </c>
+      <c r="J18" s="1">
+        <f>K18*1.5</f>
+        <v>6</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P18" s="45"/>
+    </row>
+    <row r="19" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="E19" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="K19" s="66"/>
+      <c r="P19" s="45"/>
+    </row>
+    <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="67">
+        <v>0</v>
+      </c>
+      <c r="N20" s="103"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="104"/>
+    </row>
+    <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="67">
+        <v>500</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="P21" s="69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="67">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="P22" s="69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="67">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M23" s="41"/>
+      <c r="N23" s="42"/>
+      <c r="P23" s="55"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56"/>
+      <c r="E24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="P24" s="55"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="56"/>
+      <c r="E25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="P25" s="55"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="56"/>
+      <c r="P26" s="55"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="N27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="6"/>
+      <c r="P27" s="53"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="P28" s="55"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P29" s="55"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P30" s="55"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="119"/>
+      <c r="P31" s="55"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="56"/>
+      <c r="P32" s="55"/>
+    </row>
+    <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="9">
+        <v>8</v>
+      </c>
+      <c r="E33" s="10">
+        <f>D33-1</f>
+        <v>7</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" ref="F33:L33" si="1">E33-1</f>
+        <v>6</v>
+      </c>
+      <c r="G33" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J33" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K33" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L33" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="N33" s="105"/>
+      <c r="O33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" s="53"/>
+    </row>
+    <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
+      <c r="A34" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="72">
+        <v>11</v>
+      </c>
+      <c r="D34" s="73">
+        <f>C34+1</f>
+        <v>12</v>
+      </c>
+      <c r="E34" s="72">
+        <f t="shared" ref="E34:L34" si="2">D34+1</f>
+        <v>13</v>
+      </c>
+      <c r="F34" s="73">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G34" s="72">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="H34" s="73">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="I34" s="72">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="J34" s="73">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="K34" s="72">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="L34" s="73">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M34" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="N34" s="106"/>
+      <c r="P34" s="55"/>
+    </row>
+    <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
+      <c r="A35" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="72">
+        <v>11</v>
+      </c>
+      <c r="D35" s="73">
+        <f t="shared" ref="D35:L36" si="3">C35+1</f>
+        <v>12</v>
+      </c>
+      <c r="E35" s="72">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="F35" s="73">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="G35" s="72">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="H35" s="73">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I35" s="72">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="J35" s="73">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="K35" s="72">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="L35" s="73">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="M35" s="107" t="s">
+        <v>170</v>
+      </c>
+      <c r="N35" s="107"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="55"/>
+    </row>
+    <row r="36" spans="1:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="76">
+        <v>10</v>
+      </c>
+      <c r="D36" s="77">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="E36" s="76">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="F36" s="77">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="G36" s="76">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="H36" s="77">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="I36" s="76">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="J36" s="77">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="K36" s="76">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="L36" s="77">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="M36" s="108" t="s">
+        <v>110</v>
+      </c>
+      <c r="N36" s="108"/>
+      <c r="O36" s="78"/>
+      <c r="P36" s="79"/>
+      <c r="AA36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="M8:O8"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D6BBBE-C9DF-4D21-98BF-29E96594E7D0}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:C31"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5950,7 +6874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263CECC3-3302-44DA-8376-3DD3643BBD45}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
@@ -6856,7 +7780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7F733B-4F29-4CC7-8875-78DA591CD6C7}">
   <dimension ref="A1:J76"/>
   <sheetViews>

</xml_diff>

<commit_message>
vault backup: 2025-12-17 16:44:59
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC53D759-5319-4130-8B90-038C7D8B5F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D748B98-28A3-4109-8BCD-C897764E1804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11568" yWindow="0" windowWidth="27396" windowHeight="16656" activeTab="6" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="11568" yWindow="0" windowWidth="27396" windowHeight="16656" activeTab="7" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Halfling A" sheetId="8" r:id="rId1"/>

</xml_diff>